<commit_message>
lidt nyt til tidsplanen...
</commit_message>
<xml_diff>
--- a/Modeller/Agile-Stage-Gate v0.1.xlsx
+++ b/Modeller/Agile-Stage-Gate v0.1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="25">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -44,12 +44,6 @@
     <t>Projektadministration</t>
   </si>
   <si>
-    <t>Gate: M0</t>
-  </si>
-  <si>
-    <t>Gate: M1</t>
-  </si>
-  <si>
     <t>Design</t>
   </si>
   <si>
@@ -71,7 +65,40 @@
     <t xml:space="preserve"> Gate: M3</t>
   </si>
   <si>
-    <t>Gate</t>
+    <t>Anskaffelse af HW</t>
+  </si>
+  <si>
+    <t>Anskaffelse af SW</t>
+  </si>
+  <si>
+    <t>MosCow</t>
+  </si>
+  <si>
+    <t>Tidsplan</t>
+  </si>
+  <si>
+    <t>Teoriundersøgelse</t>
+  </si>
+  <si>
+    <t>Gate: development backlog</t>
+  </si>
+  <si>
+    <t>deadline18.09.16</t>
+  </si>
+  <si>
+    <t>planlægning af litteratursøgning</t>
+  </si>
+  <si>
+    <t>litteratursøgning</t>
+  </si>
+  <si>
+    <t>high- level produktspecifikation</t>
+  </si>
+  <si>
+    <t>Gate: Produktdefinition</t>
+  </si>
+  <si>
+    <t>Planlægning af testdokumentation</t>
   </si>
 </sst>
 </file>
@@ -409,12 +436,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="135"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1382,8 +1409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="50" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1474,8 +1501,8 @@
       <c r="X4" s="27"/>
     </row>
     <row r="5" spans="1:29" ht="113.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="34"/>
-      <c r="B5" s="35"/>
+      <c r="A5" s="33"/>
+      <c r="B5" s="34"/>
       <c r="C5" s="21" t="s">
         <v>0</v>
       </c>
@@ -1560,37 +1587,35 @@
         <v>1</v>
       </c>
       <c r="C6" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="23"/>
+      <c r="F6" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="19" t="s">
+      <c r="H6" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="I6" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="J6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="24" t="s">
+      <c r="K6" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="23" t="s">
+      <c r="L6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="K6" s="19" t="s">
+      <c r="M6" s="17" t="s">
         <v>12</v>
-      </c>
-      <c r="L6" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="M6" s="17" t="s">
-        <v>14</v>
       </c>
       <c r="N6" s="7" t="s">
         <v>0</v>
@@ -1635,10 +1660,12 @@
       <c r="B7" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="9"/>
+      <c r="C7" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>21</v>
+      </c>
       <c r="E7" s="20"/>
       <c r="F7" s="15"/>
       <c r="G7" s="9"/>
@@ -1653,9 +1680,13 @@
     </row>
     <row r="8" spans="1:29" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="9"/>
+      <c r="B8" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="35"/>
+      <c r="D8" s="16" t="s">
+        <v>2</v>
+      </c>
       <c r="E8" s="9"/>
       <c r="F8" s="14"/>
       <c r="G8" s="9"/>
@@ -1669,9 +1700,13 @@
     </row>
     <row r="9" spans="1:29" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="9"/>
+      <c r="B9" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="35"/>
+      <c r="D9" s="16" t="s">
+        <v>3</v>
+      </c>
       <c r="E9" s="9"/>
       <c r="F9" s="14"/>
       <c r="G9" s="9"/>
@@ -1685,9 +1720,13 @@
     </row>
     <row r="10" spans="1:29" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="9"/>
+      <c r="B10" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="35"/>
+      <c r="D10" s="16" t="s">
+        <v>24</v>
+      </c>
       <c r="E10" s="9"/>
       <c r="F10" s="14"/>
       <c r="G10" s="9"/>
@@ -1701,8 +1740,10 @@
     </row>
     <row r="11" spans="1:29" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="33"/>
+      <c r="B11" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="35"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="14"/>
@@ -1717,8 +1758,10 @@
     </row>
     <row r="12" spans="1:29" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="33"/>
+      <c r="B12" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="35"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
       <c r="F12" s="14"/>
@@ -1733,8 +1776,10 @@
     </row>
     <row r="13" spans="1:29" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="33"/>
+      <c r="B13" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="35"/>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
       <c r="F13" s="14"/>
@@ -1750,7 +1795,7 @@
     <row r="14" spans="1:29" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="9"/>
-      <c r="C14" s="33"/>
+      <c r="C14" s="35"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
       <c r="F14" s="14"/>
@@ -1766,7 +1811,7 @@
     <row r="15" spans="1:29" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="9"/>
-      <c r="C15" s="33"/>
+      <c r="C15" s="35"/>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
       <c r="F15" s="14"/>
@@ -1782,7 +1827,7 @@
     <row r="16" spans="1:29" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="9"/>
-      <c r="C16" s="33"/>
+      <c r="C16" s="35"/>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
       <c r="F16" s="14"/>
@@ -1798,7 +1843,7 @@
     <row r="17" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="9"/>
-      <c r="C17" s="33"/>
+      <c r="C17" s="35"/>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
       <c r="F17" s="14"/>
@@ -1814,7 +1859,7 @@
     <row r="18" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="9"/>
-      <c r="C18" s="33"/>
+      <c r="C18" s="35"/>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
       <c r="F18" s="14"/>
@@ -1830,7 +1875,7 @@
     <row r="19" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="9"/>
-      <c r="C19" s="33"/>
+      <c r="C19" s="35"/>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
       <c r="F19" s="14"/>
@@ -1846,7 +1891,7 @@
     <row r="20" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="9"/>
-      <c r="C20" s="33"/>
+      <c r="C20" s="35"/>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
       <c r="F20" s="14"/>
@@ -1862,7 +1907,7 @@
     <row r="21" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="9"/>
-      <c r="C21" s="33"/>
+      <c r="C21" s="35"/>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
       <c r="F21" s="14"/>
@@ -1878,7 +1923,7 @@
     <row r="22" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="9"/>
-      <c r="C22" s="33"/>
+      <c r="C22" s="35"/>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
       <c r="F22" s="14"/>
@@ -1894,7 +1939,7 @@
     <row r="23" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="9"/>
-      <c r="C23" s="33"/>
+      <c r="C23" s="35"/>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
       <c r="F23" s="14"/>
@@ -1910,7 +1955,7 @@
     <row r="24" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="9"/>
-      <c r="C24" s="33"/>
+      <c r="C24" s="35"/>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
       <c r="F24" s="14"/>
@@ -1926,7 +1971,7 @@
     <row r="25" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="25"/>
-      <c r="C25" s="33"/>
+      <c r="C25" s="35"/>
       <c r="D25" s="25"/>
       <c r="E25" s="25"/>
       <c r="F25" s="14"/>

</xml_diff>

<commit_message>
LabView optagefrekvenssignal med loop og det hele!
</commit_message>
<xml_diff>
--- a/Modeller/Agile-Stage-Gate v0.1.xlsx
+++ b/Modeller/Agile-Stage-Gate v0.1.xlsx
@@ -41,9 +41,6 @@
     <t>AGILE-STAGE-GATE REVIEW ASSESMENT DASHBOARD</t>
   </si>
   <si>
-    <t>Projektadministration</t>
-  </si>
-  <si>
     <t>Design</t>
   </si>
   <si>
@@ -71,9 +68,6 @@
     <t>Anskaffelse af SW</t>
   </si>
   <si>
-    <t>MosCow</t>
-  </si>
-  <si>
     <t>Tidsplan</t>
   </si>
   <si>
@@ -86,19 +80,25 @@
     <t>deadline18.09.16</t>
   </si>
   <si>
-    <t>planlægning af litteratursøgning</t>
-  </si>
-  <si>
-    <t>litteratursøgning</t>
-  </si>
-  <si>
-    <t>high- level produktspecifikation</t>
-  </si>
-  <si>
     <t>Gate: Produktdefinition</t>
   </si>
   <si>
     <t>Planlægning af testdokumentation</t>
+  </si>
+  <si>
+    <t>Planlægning af litteratursøgning</t>
+  </si>
+  <si>
+    <t>High-level produktspecifikation</t>
+  </si>
+  <si>
+    <t>Litteratursøgning</t>
+  </si>
+  <si>
+    <t>MoSCoW</t>
+  </si>
+  <si>
+    <t>Samarbejdsaftale</t>
   </si>
 </sst>
 </file>
@@ -360,7 +360,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="135"/>
@@ -442,6 +442,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="45" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1410,7 +1419,7 @@
   <dimension ref="A1:AC33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1586,36 +1595,36 @@
       <c r="B6" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>22</v>
+      <c r="C6" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="38" t="s">
+        <v>21</v>
       </c>
       <c r="E6" s="23"/>
       <c r="F6" s="19" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G6" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="I6" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="24" t="s">
+      <c r="J6" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="23" t="s">
+      <c r="K6" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="K6" s="19" t="s">
+      <c r="L6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="L6" s="12" t="s">
+      <c r="M6" s="17" t="s">
         <v>11</v>
-      </c>
-      <c r="M6" s="17" t="s">
-        <v>12</v>
       </c>
       <c r="N6" s="7" t="s">
         <v>0</v>
@@ -1658,13 +1667,13 @@
     <row r="7" spans="1:29" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="16" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E7" s="20"/>
       <c r="F7" s="15"/>
@@ -1680,9 +1689,6 @@
     </row>
     <row r="8" spans="1:29" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14"/>
-      <c r="B8" s="16" t="s">
-        <v>20</v>
-      </c>
       <c r="C8" s="35"/>
       <c r="D8" s="16" t="s">
         <v>2</v>
@@ -1701,7 +1707,7 @@
     <row r="9" spans="1:29" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
       <c r="B9" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="35"/>
       <c r="D9" s="16" t="s">
@@ -1721,11 +1727,11 @@
     <row r="10" spans="1:29" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
       <c r="B10" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="35"/>
-      <c r="D10" s="16" t="s">
-        <v>24</v>
+      <c r="D10" s="36" t="s">
+        <v>19</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="14"/>
@@ -1741,7 +1747,7 @@
     <row r="11" spans="1:29" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
       <c r="B11" s="16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C11" s="35"/>
       <c r="D11" s="9"/>
@@ -1759,7 +1765,7 @@
     <row r="12" spans="1:29" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
       <c r="B12" s="16" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C12" s="35"/>
       <c r="D12" s="9"/>
@@ -1777,7 +1783,7 @@
     <row r="13" spans="1:29" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C13" s="35"/>
       <c r="D13" s="9"/>
@@ -1794,7 +1800,9 @@
     </row>
     <row r="14" spans="1:29" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
-      <c r="B14" s="9"/>
+      <c r="B14" s="36" t="s">
+        <v>20</v>
+      </c>
       <c r="C14" s="35"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>

</xml_diff>

<commit_message>
Tidsplan med agile udvilingsfase
</commit_message>
<xml_diff>
--- a/Modeller/Agile-Stage-Gate v0.1.xlsx
+++ b/Modeller/Agile-Stage-Gate v0.1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="51">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -53,33 +53,21 @@
     <t xml:space="preserve"> Opdagelser</t>
   </si>
   <si>
-    <t xml:space="preserve"> Gate: M2</t>
-  </si>
-  <si>
     <t>Implementering</t>
   </si>
   <si>
-    <t xml:space="preserve"> Gate: M3</t>
-  </si>
-  <si>
     <t>Anskaffelse af HW</t>
   </si>
   <si>
     <t>Anskaffelse af SW</t>
   </si>
   <si>
-    <t>Tidsplan</t>
-  </si>
-  <si>
     <t>Teoriundersøgelse</t>
   </si>
   <si>
     <t>Gate: development backlog</t>
   </si>
   <si>
-    <t>deadline18.09.16</t>
-  </si>
-  <si>
     <t>Gate: Produktdefinition</t>
   </si>
   <si>
@@ -99,13 +87,103 @@
   </si>
   <si>
     <t>Samarbejdsaftale</t>
+  </si>
+  <si>
+    <t>Scrumstyringsværktøj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forståelse af intented use </t>
+  </si>
+  <si>
+    <t>Tidsplaner</t>
+  </si>
+  <si>
+    <t>Reviewgruppe</t>
+  </si>
+  <si>
+    <t>deadline 18.09.16</t>
+  </si>
+  <si>
+    <t>Planlægning af testforløb</t>
+  </si>
+  <si>
+    <t>LaTeX</t>
+  </si>
+  <si>
+    <t>GitHub</t>
+  </si>
+  <si>
+    <t>Internal block diagram</t>
+  </si>
+  <si>
+    <t>Block definition diagram</t>
+  </si>
+  <si>
+    <t>HW integration</t>
+  </si>
+  <si>
+    <t>SW udvikling(LabVIEW)</t>
+  </si>
+  <si>
+    <t>SW og HW integration</t>
+  </si>
+  <si>
+    <t>Unittest</t>
+  </si>
+  <si>
+    <t>Integrationstest</t>
+  </si>
+  <si>
+    <t>Flowdiagram</t>
+  </si>
+  <si>
+    <t>Dokumentation for fund</t>
+  </si>
+  <si>
+    <t>Aktioner</t>
+  </si>
+  <si>
+    <t>Lovgivningsanalyse</t>
+  </si>
+  <si>
+    <t>deadline 02.10.16</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gate:  MVP realisering</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gate: Aflevering</t>
+  </si>
+  <si>
+    <t>deadline 16.12.16 kl. 12</t>
+  </si>
+  <si>
+    <t>Kredsløbsdiagrammer</t>
+  </si>
+  <si>
+    <t>GUI færdiggøres</t>
+  </si>
+  <si>
+    <t>SW optimering</t>
+  </si>
+  <si>
+    <t>Understøttende teori</t>
+  </si>
+  <si>
+    <t>Overvejelser omkring lovgivningsanalyse</t>
+  </si>
+  <si>
+    <t>Testopstillinger dokumenteres</t>
+  </si>
+  <si>
+    <t>Projektprocessen dokumenteres</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -150,6 +228,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -360,7 +446,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="135"/>
@@ -385,9 +471,6 @@
       <alignment textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="135"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="135"/>
     </xf>
@@ -398,7 +481,6 @@
       <alignment textRotation="135"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -408,10 +490,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="135"/>
     </xf>
@@ -446,11 +524,29 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="45" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="45" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="45" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -632,15 +728,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1619251</xdr:colOff>
+      <xdr:colOff>457200</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>266699</xdr:rowOff>
+      <xdr:rowOff>247649</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>111261</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -649,8 +745,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6324601" y="2190749"/>
-          <a:ext cx="2111510" cy="1504951"/>
+          <a:off x="5162550" y="2171699"/>
+          <a:ext cx="2114550" cy="1504951"/>
           <a:chOff x="1504951" y="2152649"/>
           <a:chExt cx="2111510" cy="1504951"/>
         </a:xfrm>
@@ -701,8 +797,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="1771650" y="2609850"/>
-            <a:ext cx="914400" cy="628650"/>
+            <a:off x="1771649" y="2609850"/>
+            <a:ext cx="1119647" cy="628650"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -732,7 +828,7 @@
           <a:p>
             <a:r>
               <a:rPr lang="da-DK" sz="1600"/>
-              <a:t>1 uge x 2 sprints</a:t>
+              <a:t>1 uge x 2 sprint</a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
@@ -785,13 +881,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>1676401</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>247649</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>168411</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
@@ -803,7 +899,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="13620751" y="2171699"/>
+          <a:off x="11811001" y="2171699"/>
           <a:ext cx="2111510" cy="1504951"/>
           <a:chOff x="1504951" y="2152649"/>
           <a:chExt cx="2111510" cy="1504951"/>
@@ -939,13 +1035,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>381001</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>247649</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>682761</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
@@ -957,7 +1053,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="19564351" y="2171699"/>
+          <a:off x="17754601" y="2171699"/>
           <a:ext cx="2111510" cy="1504951"/>
           <a:chOff x="1504951" y="2152649"/>
           <a:chExt cx="2111510" cy="1504951"/>
@@ -1089,6 +1185,222 @@
         </xdr:txBody>
       </xdr:sp>
     </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1085850</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>361950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1581150</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1114425</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Billede 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9410700" y="5448300"/>
+          <a:ext cx="5924550" cy="752475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1733550</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1295400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>885825</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1609725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Billede 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10058400" y="6381750"/>
+          <a:ext cx="962025" cy="314325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1771650</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1314450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>923925</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1628775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Billede 27"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11906250" y="6400800"/>
+          <a:ext cx="962025" cy="314325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1314450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>962025</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1628775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Billede 28"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13754100" y="6400800"/>
+          <a:ext cx="962025" cy="314325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1416,726 +1728,756 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC33"/>
+  <dimension ref="A1:AB35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="50" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.125" customWidth="1"/>
-    <col min="2" max="27" width="23.625" customWidth="1"/>
+    <col min="2" max="26" width="23.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="48.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:29" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="29"/>
-      <c r="B2" s="30" t="s">
+    <row r="1" spans="1:28" ht="48.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:28" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="25"/>
+      <c r="B2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="31"/>
-      <c r="V2" s="31"/>
-      <c r="W2" s="31"/>
-      <c r="X2" s="32"/>
-    </row>
-    <row r="3" spans="1:29" ht="68.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
-      <c r="O3" s="27"/>
-      <c r="P3" s="27"/>
-      <c r="Q3" s="27"/>
-      <c r="R3" s="27"/>
-      <c r="S3" s="27"/>
-      <c r="T3" s="27"/>
-      <c r="U3" s="27"/>
-      <c r="V3" s="27"/>
-      <c r="W3" s="27"/>
-      <c r="X3" s="27"/>
-    </row>
-    <row r="4" spans="1:29" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="27"/>
-      <c r="N4" s="27"/>
-      <c r="O4" s="27"/>
-      <c r="P4" s="27"/>
-      <c r="Q4" s="27"/>
-      <c r="R4" s="27"/>
-      <c r="S4" s="27"/>
-      <c r="T4" s="27"/>
-      <c r="U4" s="27"/>
-      <c r="V4" s="27"/>
-      <c r="W4" s="27"/>
-      <c r="X4" s="27"/>
-    </row>
-    <row r="5" spans="1:29" ht="113.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="33"/>
-      <c r="B5" s="34"/>
-      <c r="C5" s="21" t="s">
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="27"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="27"/>
+      <c r="U2" s="27"/>
+      <c r="V2" s="27"/>
+      <c r="W2" s="28"/>
+    </row>
+    <row r="3" spans="1:28" ht="68.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="23"/>
+      <c r="U3" s="23"/>
+      <c r="V3" s="23"/>
+      <c r="W3" s="23"/>
+    </row>
+    <row r="4" spans="1:28" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="22"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="23"/>
+      <c r="U4" s="23"/>
+      <c r="V4" s="23"/>
+      <c r="W4" s="23"/>
+    </row>
+    <row r="5" spans="1:28" ht="113.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="29"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="17" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="H5" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="J5" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="K5" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="M5" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="N5" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="P5" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="R5" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="S5" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="T5" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="U5" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="V5" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="W5" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="X5" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="1"/>
-      <c r="AB5" s="3"/>
-      <c r="AC5" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:29" ht="141.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="12" t="s">
+      <c r="E5" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="M5" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="S5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="U5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="V5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="W5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="X5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" ht="141.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="13"/>
+      <c r="B6" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="R6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="S6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="T6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="U6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="V6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="W6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="X6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="8"/>
+    </row>
+    <row r="7" spans="1:28" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
+      <c r="B7" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="23"/>
-      <c r="F6" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="J6" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="K6" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="L6" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="M6" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="O6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="P6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="R6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="S6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="T6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="U6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="V6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="W6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="X6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="8"/>
-    </row>
-    <row r="7" spans="1:29" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="9"/>
-      <c r="Z7" s="3"/>
-    </row>
-    <row r="8" spans="1:29" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="16" t="s">
+      <c r="E7" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="K7" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="L7" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="M7" s="9"/>
+      <c r="Y7" s="3"/>
+    </row>
+    <row r="8" spans="1:28" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
+      <c r="B8" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="31"/>
+      <c r="D8" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="9"/>
-    </row>
-    <row r="9" spans="1:29" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="35"/>
-      <c r="D9" s="16" t="s">
+      <c r="E8" s="31"/>
+      <c r="F8" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" s="31"/>
+      <c r="K8" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="L8" s="31"/>
+      <c r="M8" s="9"/>
+    </row>
+    <row r="9" spans="1:28" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
+      <c r="B9" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="31"/>
+      <c r="D9" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="32"/>
       <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="9"/>
-    </row>
-    <row r="10" spans="1:29" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="35"/>
-      <c r="D10" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="14"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="L9" s="31"/>
+      <c r="M9" s="9"/>
+    </row>
+    <row r="10" spans="1:28" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
+      <c r="B10" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="31"/>
+      <c r="D10" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="31"/>
+      <c r="F10" s="32" t="s">
+        <v>48</v>
+      </c>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="9"/>
-    </row>
-    <row r="11" spans="1:29" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="16" t="s">
+      <c r="J10" s="31"/>
+      <c r="K10" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="L10" s="31"/>
+      <c r="M10" s="9"/>
+    </row>
+    <row r="11" spans="1:28" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="13"/>
+      <c r="B11" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="31"/>
+      <c r="D11" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="14"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="9"/>
-    </row>
-    <row r="12" spans="1:29" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="35"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="L11" s="31"/>
+      <c r="M11" s="9"/>
+    </row>
+    <row r="12" spans="1:28" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="B12" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="31"/>
       <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="14"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="9"/>
-    </row>
-    <row r="13" spans="1:29" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="35"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="L12" s="31"/>
+      <c r="M12" s="9"/>
+    </row>
+    <row r="13" spans="1:28" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="13"/>
+      <c r="B13" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="31"/>
       <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="14"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="9"/>
-    </row>
-    <row r="14" spans="1:29" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="35"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="L13" s="31"/>
+      <c r="M13" s="9"/>
+    </row>
+    <row r="14" spans="1:28" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13"/>
+      <c r="B14" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="31"/>
       <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="14"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="9"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="9"/>
-    </row>
-    <row r="15" spans="1:29" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="35"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="31"/>
+      <c r="M14" s="9"/>
+    </row>
+    <row r="15" spans="1:28" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="13"/>
+      <c r="B15" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="31"/>
       <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="14"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="9"/>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="9"/>
-    </row>
-    <row r="16" spans="1:29" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="35"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="9"/>
+    </row>
+    <row r="16" spans="1:28" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="B16" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="31"/>
       <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="14"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="9"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="9"/>
-    </row>
-    <row r="17" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="35"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="9"/>
+    </row>
+    <row r="17" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
+      <c r="B17" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="31"/>
       <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="14"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="9"/>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="9"/>
-    </row>
-    <row r="18" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="35"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="31"/>
+      <c r="M17" s="9"/>
+    </row>
+    <row r="18" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
+      <c r="B18" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="31"/>
       <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="14"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="9"/>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="9"/>
-    </row>
-    <row r="19" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="31"/>
+      <c r="M18" s="9"/>
+    </row>
+    <row r="19" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
       <c r="B19" s="9"/>
-      <c r="C19" s="35"/>
+      <c r="C19" s="31"/>
       <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="14"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="9"/>
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="9"/>
-    </row>
-    <row r="20" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="31"/>
+      <c r="M19" s="9"/>
+    </row>
+    <row r="20" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
       <c r="B20" s="9"/>
-      <c r="C20" s="35"/>
+      <c r="C20" s="31"/>
       <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="14"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="9"/>
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="9"/>
-    </row>
-    <row r="21" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="31"/>
+      <c r="M20" s="9"/>
+    </row>
+    <row r="21" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
       <c r="B21" s="9"/>
-      <c r="C21" s="35"/>
+      <c r="C21" s="31"/>
       <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="14"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="9"/>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="9"/>
-    </row>
-    <row r="22" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="31"/>
+      <c r="M21" s="9"/>
+    </row>
+    <row r="22" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="13"/>
       <c r="B22" s="9"/>
-      <c r="C22" s="35"/>
+      <c r="C22" s="31"/>
       <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="14"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="9"/>
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="9"/>
-    </row>
-    <row r="23" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
+      <c r="J22" s="31"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="31"/>
+      <c r="M22" s="9"/>
+    </row>
+    <row r="23" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="13"/>
       <c r="B23" s="9"/>
-      <c r="C23" s="35"/>
+      <c r="C23" s="31"/>
       <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="14"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="9"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="9"/>
-    </row>
-    <row r="24" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
+      <c r="J23" s="31"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="31"/>
+      <c r="M23" s="9"/>
+    </row>
+    <row r="24" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="13"/>
       <c r="B24" s="9"/>
-      <c r="C24" s="35"/>
+      <c r="C24" s="31"/>
       <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="14"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="9"/>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="9"/>
-    </row>
-    <row r="25" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="25"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="25"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="25"/>
-    </row>
-    <row r="26" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="27"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="26"/>
-      <c r="K26" s="26"/>
-      <c r="L26" s="26"/>
-      <c r="M26" s="26"/>
-      <c r="N26" s="26"/>
-      <c r="O26" s="26"/>
-    </row>
-    <row r="27" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="27"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="26"/>
-      <c r="K27" s="26"/>
-      <c r="L27" s="26"/>
-      <c r="M27" s="26"/>
-      <c r="N27" s="26"/>
-      <c r="O27" s="26"/>
-    </row>
-    <row r="28" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="27"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="26"/>
-      <c r="J28" s="26"/>
-      <c r="K28" s="26"/>
-      <c r="L28" s="26"/>
-      <c r="M28" s="26"/>
-      <c r="N28" s="26"/>
-      <c r="O28" s="26"/>
-    </row>
-    <row r="29" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="27"/>
-      <c r="B29" s="26"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
-      <c r="K29" s="26"/>
-      <c r="L29" s="26"/>
-      <c r="M29" s="26"/>
-      <c r="N29" s="26"/>
-      <c r="O29" s="26"/>
-    </row>
-    <row r="30" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="27"/>
-      <c r="B30" s="26"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
-      <c r="K30" s="26"/>
-      <c r="L30" s="26"/>
-      <c r="M30" s="26"/>
-      <c r="N30" s="26"/>
-      <c r="O30" s="26"/>
-    </row>
-    <row r="31" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="27"/>
-      <c r="B31" s="26"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="26"/>
-      <c r="K31" s="26"/>
-      <c r="L31" s="26"/>
-      <c r="M31" s="26"/>
-      <c r="N31" s="26"/>
-      <c r="O31" s="26"/>
-    </row>
-    <row r="32" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="27"/>
-      <c r="B32" s="27"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="26"/>
-      <c r="H32" s="26"/>
-      <c r="I32" s="26"/>
-      <c r="J32" s="26"/>
-      <c r="K32" s="26"/>
-      <c r="L32" s="26"/>
-      <c r="M32" s="26"/>
-      <c r="N32" s="26"/>
-      <c r="O32" s="26"/>
-    </row>
-    <row r="33" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="27"/>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="26"/>
-      <c r="H33" s="26"/>
-      <c r="I33" s="26"/>
-      <c r="J33" s="26"/>
-      <c r="K33" s="26"/>
-      <c r="L33" s="26"/>
-      <c r="M33" s="26"/>
-      <c r="N33" s="26"/>
-      <c r="O33" s="26"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="31"/>
+      <c r="M24" s="9"/>
+    </row>
+    <row r="25" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="13"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="31"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="31"/>
+      <c r="M25" s="21"/>
+    </row>
+    <row r="26" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="23"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="22"/>
+      <c r="L26" s="22"/>
+      <c r="M26" s="22"/>
+      <c r="N26" s="22"/>
+    </row>
+    <row r="27" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="23"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="22"/>
+      <c r="M27" s="22"/>
+      <c r="N27" s="22"/>
+    </row>
+    <row r="28" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="23"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
+      <c r="L28" s="22"/>
+      <c r="M28" s="22"/>
+      <c r="N28" s="22"/>
+    </row>
+    <row r="29" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="23"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="22"/>
+      <c r="J29" s="22"/>
+      <c r="K29" s="22"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="22"/>
+      <c r="N29" s="22"/>
+    </row>
+    <row r="30" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="23"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="22"/>
+      <c r="L30" s="22"/>
+      <c r="M30" s="22"/>
+      <c r="N30" s="22"/>
+    </row>
+    <row r="31" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="23"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="22"/>
+      <c r="L31" s="22"/>
+      <c r="M31" s="22"/>
+      <c r="N31" s="22"/>
+    </row>
+    <row r="32" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="23"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="22"/>
+      <c r="J32" s="22"/>
+      <c r="K32" s="22"/>
+      <c r="L32" s="22"/>
+      <c r="M32" s="22"/>
+      <c r="N32" s="22"/>
+    </row>
+    <row r="33" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="23"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22"/>
+      <c r="K33" s="22"/>
+      <c r="L33" s="22"/>
+      <c r="M33" s="22"/>
+      <c r="N33" s="22"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B34" s="23"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B35" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
+    <mergeCell ref="L7:L25"/>
     <mergeCell ref="C7:C25"/>
+    <mergeCell ref="E7:E25"/>
+    <mergeCell ref="J7:J25"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Stage gate model færdig!
</commit_message>
<xml_diff>
--- a/Modeller/Agile-Stage-Gate v0.1.xlsx
+++ b/Modeller/Agile-Stage-Gate v0.1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="71">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -41,6 +41,9 @@
     <t>AGILE-STAGE-GATE REVIEW ASSESMENT DASHBOARD</t>
   </si>
   <si>
+    <t>Projektadministration</t>
+  </si>
+  <si>
     <t>Design</t>
   </si>
   <si>
@@ -177,13 +180,70 @@
   </si>
   <si>
     <t>Projektprocessen dokumenteres</t>
+  </si>
+  <si>
+    <t>Resumé</t>
+  </si>
+  <si>
+    <t>Projektrapport</t>
+  </si>
+  <si>
+    <t>Procesrapport</t>
+  </si>
+  <si>
+    <t>Indledning</t>
+  </si>
+  <si>
+    <t>Problemformulering</t>
+  </si>
+  <si>
+    <t>Metoder</t>
+  </si>
+  <si>
+    <t>Resultater</t>
+  </si>
+  <si>
+    <t>Diskussion</t>
+  </si>
+  <si>
+    <t>Konklusion</t>
+  </si>
+  <si>
+    <t>Perspektivering</t>
+  </si>
+  <si>
+    <t>Testprotokol</t>
+  </si>
+  <si>
+    <t>Projektstyrings-værktøjer</t>
+  </si>
+  <si>
+    <t>Udviklingsværktøjer</t>
+  </si>
+  <si>
+    <t>Opnåede erfaringer</t>
+  </si>
+  <si>
+    <t>Logbog</t>
+  </si>
+  <si>
+    <t>Intern/ ekstern kommunikation</t>
+  </si>
+  <si>
+    <t>deadline 09.12.16</t>
+  </si>
+  <si>
+    <t>Dokumentations-rapport</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gate: empirisk sammenfatning</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -235,6 +295,13 @@
     <font>
       <b/>
       <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -446,7 +513,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="135"/>
@@ -455,21 +522,6 @@
       <alignment textRotation="135"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="135"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="135"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="135"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="45"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="135"/>
@@ -502,7 +554,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -547,6 +598,31 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="45" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -591,8 +667,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1504951" y="2171699"/>
-          <a:ext cx="2111510" cy="1504951"/>
+          <a:off x="1490664" y="2152649"/>
+          <a:ext cx="2111510" cy="1509714"/>
           <a:chOff x="1504951" y="2152649"/>
           <a:chExt cx="2111510" cy="1504951"/>
         </a:xfrm>
@@ -745,8 +821,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5162550" y="2171699"/>
-          <a:ext cx="2114550" cy="1504951"/>
+          <a:off x="5148263" y="2152649"/>
+          <a:ext cx="2114550" cy="1509714"/>
           <a:chOff x="1504951" y="2152649"/>
           <a:chExt cx="2111510" cy="1504951"/>
         </a:xfrm>
@@ -899,8 +975,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="11811001" y="2171699"/>
-          <a:ext cx="2111510" cy="1504951"/>
+          <a:off x="11796714" y="2152649"/>
+          <a:ext cx="2111510" cy="1509714"/>
           <a:chOff x="1504951" y="2152649"/>
           <a:chExt cx="2111510" cy="1504951"/>
         </a:xfrm>
@@ -1053,8 +1129,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="17754601" y="2171699"/>
-          <a:ext cx="2111510" cy="1504951"/>
+          <a:off x="17740314" y="2152649"/>
+          <a:ext cx="2111510" cy="1509714"/>
           <a:chOff x="1504951" y="2152649"/>
           <a:chExt cx="2111510" cy="1504951"/>
         </a:xfrm>
@@ -1401,6 +1477,160 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1057258</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>257177</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>1359018</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>28578</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="30" name="Gruppe 29"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="23845821" y="2162177"/>
+          <a:ext cx="2111510" cy="1509714"/>
+          <a:chOff x="1504951" y="2152649"/>
+          <a:chExt cx="2111510" cy="1504951"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="31" name="Billede 30"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+            <a:clrChange>
+              <a:clrFrom>
+                <a:srgbClr val="FFFFFF"/>
+              </a:clrFrom>
+              <a:clrTo>
+                <a:srgbClr val="FFFFFF">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:clrTo>
+            </a:clrChange>
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1504951" y="2152649"/>
+            <a:ext cx="2111510" cy="1504951"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="32" name="Tekstfelt 31"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1771650" y="2609850"/>
+            <a:ext cx="914400" cy="628650"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="da-DK" sz="1600"/>
+              <a:t>1 uge x 2 sprints</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="33" name="Tekstfelt 32"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2819400" y="2305050"/>
+            <a:ext cx="590550" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="da-DK" sz="1600"/>
+              <a:t>24 t</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1728,751 +1958,692 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB35"/>
+  <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="E7" zoomScale="40" zoomScaleNormal="40" zoomScalePageLayoutView="50" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.125" customWidth="1"/>
-    <col min="2" max="26" width="23.625" customWidth="1"/>
+    <col min="2" max="18" width="23.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="48.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:28" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="26" t="s">
+    <row r="1" spans="1:20" ht="48.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:20" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19"/>
+      <c r="B2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="27"/>
-      <c r="V2" s="27"/>
-      <c r="W2" s="28"/>
-    </row>
-    <row r="3" spans="1:28" ht="68.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="23"/>
-      <c r="Q3" s="23"/>
-      <c r="R3" s="23"/>
-      <c r="S3" s="23"/>
-      <c r="T3" s="23"/>
-      <c r="U3" s="23"/>
-      <c r="V3" s="23"/>
-      <c r="W3" s="23"/>
-    </row>
-    <row r="4" spans="1:28" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
-      <c r="N4" s="23"/>
-      <c r="O4" s="23"/>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="23"/>
-      <c r="R4" s="23"/>
-      <c r="S4" s="23"/>
-      <c r="T4" s="23"/>
-      <c r="U4" s="23"/>
-      <c r="V4" s="23"/>
-      <c r="W4" s="23"/>
-    </row>
-    <row r="5" spans="1:28" ht="113.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="17" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="22"/>
+    </row>
+    <row r="3" spans="1:20" ht="68.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17"/>
+    </row>
+    <row r="4" spans="1:20" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
+    </row>
+    <row r="5" spans="1:20" ht="113.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="23"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="K5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="L5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="M5" s="10" t="s">
+      <c r="M5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="O5" s="6" t="s">
+      <c r="Q5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="R5" s="1"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="Q5" s="6" t="s">
+    </row>
+    <row r="6" spans="1:20" ht="141.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="B6" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L6" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="M6" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="N6" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="O6" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="P6" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q6" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="R5" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="S5" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="T5" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="U5" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="V5" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="W5" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="X5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="1"/>
-      <c r="AA5" s="3"/>
-      <c r="AB5" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" ht="141.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="37" t="s">
+      <c r="R6" s="3"/>
+    </row>
+    <row r="7" spans="1:20" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="L7" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="M7" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="N7" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="O7" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="P7" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q7" s="41"/>
+    </row>
+    <row r="8" spans="1:20" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="25"/>
+      <c r="D8" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="25"/>
+      <c r="F8" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="J8" s="25"/>
+      <c r="K8" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="L8" s="25"/>
+      <c r="M8" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="N8" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="O8" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="P8" s="25"/>
+    </row>
+    <row r="9" spans="1:20" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="25"/>
+      <c r="D9" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="25"/>
+      <c r="F9" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="26"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="L9" s="25"/>
+      <c r="M9" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="N9" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="O9" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="P9" s="25"/>
+    </row>
+    <row r="10" spans="1:20" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="25"/>
+      <c r="D10" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="25"/>
+      <c r="F10" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="L10" s="25"/>
+      <c r="M10" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="N10" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="O10" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="P10" s="25"/>
+    </row>
+    <row r="11" spans="1:20" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="25"/>
+      <c r="D11" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="25"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="L11" s="25"/>
+      <c r="M11" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="N11" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="O11" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="P11" s="25"/>
+    </row>
+    <row r="12" spans="1:20" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="25"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="L12" s="25"/>
+      <c r="M12" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="N12" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="O12" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="P12" s="25"/>
+    </row>
+    <row r="13" spans="1:20" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="25"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="L13" s="25"/>
+      <c r="M13" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="N13" s="37"/>
+      <c r="O13" s="37"/>
+      <c r="P13" s="25"/>
+    </row>
+    <row r="14" spans="1:20" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="B14" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="25"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="25"/>
+      <c r="M14" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="N14" s="4"/>
+      <c r="O14" s="37"/>
+      <c r="P14" s="25"/>
+    </row>
+    <row r="15" spans="1:20" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="25"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="25"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="37"/>
+      <c r="P15" s="25"/>
+    </row>
+    <row r="16" spans="1:20" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="J6" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="K6" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="L6" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="O6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="P6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="R6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="S6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="T6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="U6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="V6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="W6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="X6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="8"/>
-    </row>
-    <row r="7" spans="1:28" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="I7" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="J7" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="K7" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="L7" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="M7" s="9"/>
-      <c r="Y7" s="3"/>
-    </row>
-    <row r="8" spans="1:28" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="31"/>
-      <c r="D8" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="31"/>
-      <c r="F8" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="H8" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="I8" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="J8" s="31"/>
-      <c r="K8" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="L8" s="31"/>
-      <c r="M8" s="9"/>
-    </row>
-    <row r="9" spans="1:28" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="31"/>
-      <c r="D9" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="31"/>
-      <c r="F9" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="H9" s="32"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="L9" s="31"/>
-      <c r="M9" s="9"/>
-    </row>
-    <row r="10" spans="1:28" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="31"/>
-      <c r="F10" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="L10" s="31"/>
-      <c r="M10" s="9"/>
-    </row>
-    <row r="11" spans="1:28" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="31"/>
-      <c r="D11" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="31"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="L11" s="31"/>
-      <c r="M11" s="9"/>
-    </row>
-    <row r="12" spans="1:28" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="31"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="L12" s="31"/>
-      <c r="M12" s="9"/>
-    </row>
-    <row r="13" spans="1:28" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="14" t="s">
+      <c r="C16" s="25"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="37"/>
+      <c r="P16" s="25"/>
+    </row>
+    <row r="17" spans="1:16" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="25"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="25"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="25"/>
+    </row>
+    <row r="18" spans="1:16" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="31"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="L13" s="31"/>
-      <c r="M13" s="9"/>
-    </row>
-    <row r="14" spans="1:28" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="31"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="31"/>
-      <c r="M14" s="9"/>
-    </row>
-    <row r="15" spans="1:28" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="38" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="31"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="31"/>
-      <c r="M15" s="9"/>
-    </row>
-    <row r="16" spans="1:28" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="31"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="31"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="31"/>
-      <c r="M16" s="9"/>
-    </row>
-    <row r="17" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="31"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="31"/>
-      <c r="M17" s="9"/>
-    </row>
-    <row r="18" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="31"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="31"/>
-      <c r="M18" s="9"/>
-    </row>
-    <row r="19" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="31"/>
-      <c r="M19" s="9"/>
-    </row>
-    <row r="20" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="31"/>
-      <c r="M20" s="9"/>
-    </row>
-    <row r="21" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="31"/>
-      <c r="M21" s="9"/>
-    </row>
-    <row r="22" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="31"/>
-      <c r="M22" s="9"/>
-    </row>
-    <row r="23" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="31"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="31"/>
-      <c r="M23" s="9"/>
-    </row>
-    <row r="24" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="31"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="31"/>
-      <c r="M24" s="9"/>
-    </row>
-    <row r="25" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21"/>
-      <c r="J25" s="31"/>
-      <c r="K25" s="21"/>
-      <c r="L25" s="31"/>
-      <c r="M25" s="21"/>
-    </row>
-    <row r="26" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="23"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="22"/>
-      <c r="K26" s="22"/>
-      <c r="L26" s="22"/>
-      <c r="M26" s="22"/>
-      <c r="N26" s="22"/>
-    </row>
-    <row r="27" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="23"/>
-      <c r="B27" s="21"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
-      <c r="K27" s="22"/>
-      <c r="L27" s="22"/>
-      <c r="M27" s="22"/>
-      <c r="N27" s="22"/>
-    </row>
-    <row r="28" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22"/>
-      <c r="K28" s="22"/>
-      <c r="L28" s="22"/>
-      <c r="M28" s="22"/>
-      <c r="N28" s="22"/>
-    </row>
-    <row r="29" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="23"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="22"/>
-      <c r="J29" s="22"/>
-      <c r="K29" s="22"/>
-      <c r="L29" s="22"/>
-      <c r="M29" s="22"/>
-      <c r="N29" s="22"/>
-    </row>
-    <row r="30" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="23"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="22"/>
-      <c r="J30" s="22"/>
-      <c r="K30" s="22"/>
-      <c r="L30" s="22"/>
-      <c r="M30" s="22"/>
-      <c r="N30" s="22"/>
-    </row>
-    <row r="31" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="23"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="22"/>
-      <c r="J31" s="22"/>
-      <c r="K31" s="22"/>
-      <c r="L31" s="22"/>
-      <c r="M31" s="22"/>
-      <c r="N31" s="22"/>
-    </row>
-    <row r="32" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="23"/>
-      <c r="B32" s="22"/>
-      <c r="C32" s="23"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="22"/>
-      <c r="J32" s="22"/>
-      <c r="K32" s="22"/>
-      <c r="L32" s="22"/>
-      <c r="M32" s="22"/>
-      <c r="N32" s="22"/>
-    </row>
-    <row r="33" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="23"/>
-      <c r="B33" s="22"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="22"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="22"/>
-      <c r="I33" s="22"/>
-      <c r="J33" s="22"/>
-      <c r="K33" s="22"/>
-      <c r="L33" s="22"/>
-      <c r="M33" s="22"/>
-      <c r="N33" s="22"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B34" s="23"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B35" s="23"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="25"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="25"/>
+    </row>
+    <row r="19" spans="1:16" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="25"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="25"/>
+    </row>
+    <row r="20" spans="1:16" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="25"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="25"/>
+    </row>
+    <row r="21" spans="1:16" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="25"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="25"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="25"/>
+    </row>
+    <row r="22" spans="1:16" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="17"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="16"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="16"/>
+      <c r="P22" s="16"/>
+    </row>
+    <row r="23" spans="1:16" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="17"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="16"/>
+    </row>
+    <row r="24" spans="1:16" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="17"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="16"/>
+      <c r="O24" s="16"/>
+      <c r="P24" s="16"/>
+    </row>
+    <row r="25" spans="1:16" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="17"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="16"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="16"/>
+    </row>
+    <row r="26" spans="1:16" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="17"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="16"/>
+      <c r="N26" s="16"/>
+      <c r="O26" s="16"/>
+      <c r="P26" s="16"/>
+    </row>
+    <row r="27" spans="1:16" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="17"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="16"/>
+      <c r="O27" s="16"/>
+      <c r="P27" s="16"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B28" s="17"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B29" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="L7:L25"/>
-    <mergeCell ref="C7:C25"/>
-    <mergeCell ref="E7:E25"/>
-    <mergeCell ref="J7:J25"/>
+  <mergeCells count="5">
+    <mergeCell ref="L7:L21"/>
+    <mergeCell ref="P7:P21"/>
+    <mergeCell ref="C7:C21"/>
+    <mergeCell ref="E7:E21"/>
+    <mergeCell ref="J7:J21"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Opdateret stage gate - nu med sprints der passer
</commit_message>
<xml_diff>
--- a/Modeller/Agile-Stage-Gate v0.1.xlsx
+++ b/Modeller/Agile-Stage-Gate v0.1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="73">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -237,6 +237,12 @@
   </si>
   <si>
     <t xml:space="preserve"> Gate: empirisk sammenfatning</t>
+  </si>
+  <si>
+    <t>Review med SAT 09.12.2016</t>
+  </si>
+  <si>
+    <t>Review 12.12.2016</t>
   </si>
 </sst>
 </file>
@@ -308,7 +314,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -324,6 +330,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFAF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -513,7 +525,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="135"/>
@@ -569,9 +581,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="135"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -596,9 +605,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="45"/>
     </xf>
@@ -610,9 +616,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
@@ -623,6 +626,32 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="135"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="135"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -634,6 +663,16 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFFAF"/>
+      <color rgb="FFFFFF99"/>
+      <color rgb="FF9DB99D"/>
+      <color rgb="FF0099FF"/>
+      <color rgb="FF3366CC"/>
+      <color rgb="FF0066CC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -904,7 +943,13 @@
           <a:p>
             <a:r>
               <a:rPr lang="da-DK" sz="1600"/>
-              <a:t>1 uge x 2 sprint</a:t>
+              <a:t>1 uge x</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="da-DK" sz="1600"/>
+              <a:t>2 sprint</a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
@@ -1058,7 +1103,7 @@
           <a:p>
             <a:r>
               <a:rPr lang="da-DK" sz="1600"/>
-              <a:t>1 uge x 2 sprints</a:t>
+              <a:t>1 uge x 9 sprints</a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
@@ -1212,7 +1257,15 @@
           <a:p>
             <a:r>
               <a:rPr lang="da-DK" sz="1600"/>
-              <a:t>1 uge x 2 sprints</a:t>
+              <a:t>1 uge x 1</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="da-DK" sz="1600" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="da-DK" sz="1600"/>
+              <a:t>sprints</a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
@@ -1481,13 +1534,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>1057258</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>257177</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>1359018</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>28578</xdr:rowOff>
@@ -1499,7 +1552,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="23845821" y="2162177"/>
+          <a:off x="25655571" y="2162177"/>
           <a:ext cx="2111510" cy="1509714"/>
           <a:chOff x="1504951" y="2152649"/>
           <a:chExt cx="2111510" cy="1504951"/>
@@ -1582,7 +1635,15 @@
           <a:p>
             <a:r>
               <a:rPr lang="da-DK" sz="1600"/>
-              <a:t>1 uge x 2 sprints</a:t>
+              <a:t>1 uge x 1</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="da-DK" sz="1600" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="da-DK" sz="1600"/>
+              <a:t>sprints</a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
@@ -1958,20 +2019,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T29"/>
+  <dimension ref="A1:V29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E7" zoomScale="40" zoomScaleNormal="40" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="40" zoomScaleNormal="40" zoomScalePageLayoutView="50" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.125" customWidth="1"/>
-    <col min="2" max="18" width="23.625" customWidth="1"/>
+    <col min="2" max="12" width="23.625" customWidth="1"/>
+    <col min="13" max="13" width="23.625" style="17" customWidth="1"/>
+    <col min="14" max="16" width="23.625" customWidth="1"/>
+    <col min="17" max="17" width="23.625" style="17" customWidth="1"/>
+    <col min="18" max="20" width="23.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="48.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:20" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="48.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:22" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19"/>
       <c r="B2" s="20" t="s">
         <v>4</v>
@@ -1990,9 +2055,11 @@
       <c r="N2" s="21"/>
       <c r="O2" s="21"/>
       <c r="P2" s="21"/>
-      <c r="Q2" s="22"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
+      <c r="S2" s="22"/>
     </row>
-    <row r="3" spans="1:20" ht="68.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" ht="68.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17"/>
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
@@ -2005,13 +2072,13 @@
       <c r="J3" s="17"/>
       <c r="K3" s="17"/>
       <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
       <c r="N3" s="17"/>
       <c r="O3" s="17"/>
       <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
+      <c r="R3" s="17"/>
+      <c r="S3" s="17"/>
     </row>
-    <row r="4" spans="1:20" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16"/>
       <c r="B4" s="17"/>
       <c r="C4" s="17"/>
@@ -2024,13 +2091,13 @@
       <c r="J4" s="17"/>
       <c r="K4" s="17"/>
       <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
       <c r="N4" s="17"/>
       <c r="O4" s="17"/>
       <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="17"/>
     </row>
-    <row r="5" spans="1:20" ht="113.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" ht="113.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="23"/>
       <c r="B5" s="24"/>
       <c r="C5" s="12" t="s">
@@ -2063,35 +2130,37 @@
       <c r="L5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="M5" s="5"/>
+      <c r="N5" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="N5" s="7"/>
       <c r="O5" s="7"/>
-      <c r="P5" s="7" t="s">
+      <c r="P5" s="7"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="Q5" s="5" t="s">
+      <c r="S5" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="R5" s="1"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="2" t="s">
+      <c r="T5" s="1"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="141.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" ht="141.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="27" t="s">
         <v>14</v>
       </c>
       <c r="F6" s="11" t="s">
@@ -2106,442 +2175,480 @@
       <c r="I6" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="33" t="s">
+      <c r="J6" s="32" t="s">
         <v>42</v>
       </c>
       <c r="K6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L6" s="42" t="s">
+      <c r="L6" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="M6" s="35" t="s">
+      <c r="M6" s="43"/>
+      <c r="N6" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="N6" s="43" t="s">
+      <c r="O6" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="O6" s="36" t="s">
+      <c r="P6" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="P6" s="10" t="s">
+      <c r="Q6" s="43"/>
+      <c r="R6" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="Q6" s="40" t="s">
+      <c r="S6" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="R6" s="3"/>
+      <c r="T6" s="3"/>
     </row>
-    <row r="7" spans="1:20" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="42" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="26" t="s">
+      <c r="G7" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="26" t="s">
+      <c r="H7" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="I7" s="26" t="s">
+      <c r="I7" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="J7" s="34" t="s">
+      <c r="J7" s="41" t="s">
         <v>41</v>
       </c>
       <c r="K7" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="L7" s="34" t="s">
+      <c r="L7" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="M7" s="37" t="s">
+      <c r="M7" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="N7" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="N7" s="37" t="s">
+      <c r="O7" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="O7" s="37" t="s">
+      <c r="P7" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="P7" s="39" t="s">
+      <c r="Q7" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="R7" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="Q7" s="41"/>
+      <c r="S7" s="38"/>
     </row>
-    <row r="8" spans="1:20" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="25"/>
+      <c r="C8" s="42"/>
       <c r="D8" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="25"/>
-      <c r="F8" s="26" t="s">
+      <c r="E8" s="42"/>
+      <c r="F8" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="26" t="s">
+      <c r="G8" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="H8" s="26" t="s">
+      <c r="H8" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="I8" s="26" t="s">
+      <c r="I8" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="25"/>
-      <c r="K8" s="26" t="s">
+      <c r="J8" s="42"/>
+      <c r="K8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="L8" s="25"/>
-      <c r="M8" s="37" t="s">
+      <c r="L8" s="42"/>
+      <c r="M8" s="46"/>
+      <c r="N8" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="N8" s="37" t="s">
+      <c r="O8" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="O8" s="38" t="s">
+      <c r="P8" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="P8" s="25"/>
+      <c r="Q8" s="46"/>
+      <c r="R8" s="47"/>
     </row>
-    <row r="9" spans="1:20" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="25"/>
+      <c r="C9" s="42"/>
       <c r="D9" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="26" t="s">
+      <c r="E9" s="42"/>
+      <c r="F9" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="G9" s="26" t="s">
+      <c r="G9" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="26"/>
+      <c r="H9" s="25"/>
       <c r="I9" s="4"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="26" t="s">
+      <c r="J9" s="42"/>
+      <c r="K9" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="L9" s="25"/>
-      <c r="M9" s="37" t="s">
+      <c r="L9" s="42"/>
+      <c r="M9" s="46"/>
+      <c r="N9" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="N9" s="37" t="s">
+      <c r="O9" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="O9" s="37" t="s">
+      <c r="P9" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="P9" s="25"/>
+      <c r="Q9" s="46"/>
+      <c r="R9" s="47"/>
     </row>
-    <row r="10" spans="1:20" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="26" t="s">
+      <c r="C10" s="42"/>
+      <c r="D10" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="25"/>
-      <c r="F10" s="26" t="s">
+      <c r="E10" s="42"/>
+      <c r="F10" s="25" t="s">
         <v>49</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="26" t="s">
+      <c r="J10" s="42"/>
+      <c r="K10" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="L10" s="25"/>
-      <c r="M10" s="37" t="s">
+      <c r="L10" s="42"/>
+      <c r="M10" s="46"/>
+      <c r="N10" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="N10" s="37" t="s">
+      <c r="O10" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="O10" s="37" t="s">
+      <c r="P10" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="P10" s="25"/>
+      <c r="Q10" s="46"/>
+      <c r="R10" s="47"/>
     </row>
-    <row r="11" spans="1:20" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="26" t="s">
+      <c r="C11" s="42"/>
+      <c r="D11" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="25"/>
+      <c r="E11" s="42"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="26" t="s">
+      <c r="J11" s="42"/>
+      <c r="K11" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="L11" s="25"/>
-      <c r="M11" s="37" t="s">
+      <c r="L11" s="42"/>
+      <c r="M11" s="46"/>
+      <c r="N11" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="N11" s="37" t="s">
+      <c r="O11" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="O11" s="37" t="s">
+      <c r="P11" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="P11" s="25"/>
+      <c r="Q11" s="46"/>
+      <c r="R11" s="47"/>
     </row>
-    <row r="12" spans="1:20" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="25"/>
+      <c r="C12" s="42"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="25"/>
+      <c r="E12" s="42"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="26" t="s">
+      <c r="J12" s="42"/>
+      <c r="K12" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="L12" s="25"/>
-      <c r="M12" s="37" t="s">
+      <c r="L12" s="42"/>
+      <c r="M12" s="46"/>
+      <c r="N12" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="N12" s="37" t="s">
+      <c r="O12" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="O12" s="38" t="s">
+      <c r="P12" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="P12" s="25"/>
+      <c r="Q12" s="46"/>
+      <c r="R12" s="47"/>
     </row>
-    <row r="13" spans="1:20" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="25"/>
+      <c r="C13" s="42"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="25"/>
+      <c r="E13" s="42"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="26" t="s">
+      <c r="J13" s="42"/>
+      <c r="K13" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="L13" s="25"/>
-      <c r="M13" s="37" t="s">
+      <c r="L13" s="42"/>
+      <c r="M13" s="46"/>
+      <c r="N13" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="N13" s="37"/>
-      <c r="O13" s="37"/>
-      <c r="P13" s="25"/>
+      <c r="O13" s="35"/>
+      <c r="P13" s="35"/>
+      <c r="Q13" s="46"/>
+      <c r="R13" s="47"/>
     </row>
-    <row r="14" spans="1:20" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="25"/>
+      <c r="C14" s="42"/>
       <c r="D14" s="4"/>
-      <c r="E14" s="25"/>
+      <c r="E14" s="42"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
-      <c r="J14" s="25"/>
+      <c r="J14" s="42"/>
       <c r="K14" s="4"/>
-      <c r="L14" s="25"/>
-      <c r="M14" s="37" t="s">
+      <c r="L14" s="42"/>
+      <c r="M14" s="46"/>
+      <c r="N14" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="N14" s="4"/>
-      <c r="O14" s="37"/>
-      <c r="P14" s="25"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="35"/>
+      <c r="Q14" s="46"/>
+      <c r="R14" s="47"/>
     </row>
-    <row r="15" spans="1:20" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="25"/>
+      <c r="C15" s="42"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="25"/>
+      <c r="E15" s="42"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
-      <c r="J15" s="25"/>
+      <c r="J15" s="42"/>
       <c r="K15" s="4"/>
-      <c r="L15" s="25"/>
-      <c r="M15" s="4"/>
+      <c r="L15" s="42"/>
+      <c r="M15" s="46"/>
       <c r="N15" s="4"/>
-      <c r="O15" s="37"/>
-      <c r="P15" s="25"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="35"/>
+      <c r="Q15" s="46"/>
+      <c r="R15" s="47"/>
     </row>
-    <row r="16" spans="1:20" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="25"/>
+      <c r="C16" s="42"/>
       <c r="D16" s="4"/>
-      <c r="E16" s="25"/>
+      <c r="E16" s="42"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
-      <c r="J16" s="25"/>
+      <c r="J16" s="42"/>
       <c r="K16" s="4"/>
-      <c r="L16" s="25"/>
-      <c r="M16" s="4"/>
+      <c r="L16" s="42"/>
+      <c r="M16" s="46"/>
       <c r="N16" s="4"/>
-      <c r="O16" s="37"/>
-      <c r="P16" s="25"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="35"/>
+      <c r="Q16" s="46"/>
+      <c r="R16" s="47"/>
     </row>
-    <row r="17" spans="1:16" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="25"/>
+      <c r="C17" s="42"/>
       <c r="D17" s="4"/>
-      <c r="E17" s="25"/>
+      <c r="E17" s="42"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
-      <c r="J17" s="25"/>
+      <c r="J17" s="42"/>
       <c r="K17" s="4"/>
-      <c r="L17" s="25"/>
-      <c r="M17" s="4"/>
+      <c r="L17" s="42"/>
+      <c r="M17" s="46"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
-      <c r="P17" s="25"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="46"/>
+      <c r="R17" s="47"/>
     </row>
-    <row r="18" spans="1:16" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="25"/>
+      <c r="C18" s="42"/>
       <c r="D18" s="4"/>
-      <c r="E18" s="25"/>
+      <c r="E18" s="42"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
-      <c r="J18" s="25"/>
+      <c r="J18" s="42"/>
       <c r="K18" s="4"/>
-      <c r="L18" s="25"/>
-      <c r="M18" s="4"/>
+      <c r="L18" s="42"/>
+      <c r="M18" s="46"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
-      <c r="P18" s="25"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="46"/>
+      <c r="R18" s="47"/>
     </row>
-    <row r="19" spans="1:16" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="4"/>
-      <c r="C19" s="25"/>
+      <c r="C19" s="42"/>
       <c r="D19" s="4"/>
-      <c r="E19" s="25"/>
+      <c r="E19" s="42"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
-      <c r="J19" s="25"/>
+      <c r="J19" s="42"/>
       <c r="K19" s="4"/>
-      <c r="L19" s="25"/>
-      <c r="M19" s="4"/>
+      <c r="L19" s="42"/>
+      <c r="M19" s="46"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
-      <c r="P19" s="25"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="46"/>
+      <c r="R19" s="47"/>
     </row>
-    <row r="20" spans="1:16" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="4"/>
-      <c r="C20" s="25"/>
+      <c r="C20" s="42"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="25"/>
+      <c r="E20" s="42"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
-      <c r="J20" s="25"/>
+      <c r="J20" s="42"/>
       <c r="K20" s="4"/>
-      <c r="L20" s="25"/>
-      <c r="M20" s="4"/>
+      <c r="L20" s="42"/>
+      <c r="M20" s="46"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
-      <c r="P20" s="25"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="46"/>
+      <c r="R20" s="47"/>
     </row>
-    <row r="21" spans="1:16" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="25"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
-      <c r="P21" s="25"/>
+      <c r="B21" s="48"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="48"/>
+      <c r="I21" s="48"/>
+      <c r="J21" s="42"/>
+      <c r="K21" s="48"/>
+      <c r="L21" s="42"/>
+      <c r="M21" s="46"/>
+      <c r="N21" s="48"/>
+      <c r="O21" s="48"/>
+      <c r="P21" s="48"/>
+      <c r="Q21" s="46"/>
+      <c r="R21" s="47"/>
     </row>
-    <row r="22" spans="1:16" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="16"/>
-      <c r="L22" s="16"/>
-      <c r="M22" s="16"/>
-      <c r="N22" s="16"/>
-      <c r="O22" s="16"/>
-      <c r="P22" s="16"/>
+    <row r="22" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="49"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="49"/>
+      <c r="G22" s="49"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="49"/>
+      <c r="L22" s="49"/>
+      <c r="M22" s="49"/>
+      <c r="N22" s="49"/>
+      <c r="O22" s="49"/>
+      <c r="P22" s="49"/>
+      <c r="Q22" s="49"/>
+      <c r="R22" s="49"/>
     </row>
-    <row r="23" spans="1:16" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17"/>
       <c r="B23" s="16"/>
       <c r="C23" s="18"/>
@@ -2558,8 +2665,10 @@
       <c r="N23" s="16"/>
       <c r="O23" s="16"/>
       <c r="P23" s="16"/>
+      <c r="Q23" s="16"/>
+      <c r="R23" s="16"/>
     </row>
-    <row r="24" spans="1:16" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="17"/>
       <c r="B24" s="16"/>
       <c r="C24" s="18"/>
@@ -2576,8 +2685,10 @@
       <c r="N24" s="16"/>
       <c r="O24" s="16"/>
       <c r="P24" s="16"/>
+      <c r="Q24" s="16"/>
+      <c r="R24" s="16"/>
     </row>
-    <row r="25" spans="1:16" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="17"/>
       <c r="B25" s="16"/>
       <c r="C25" s="18"/>
@@ -2594,8 +2705,10 @@
       <c r="N25" s="16"/>
       <c r="O25" s="16"/>
       <c r="P25" s="16"/>
+      <c r="Q25" s="16"/>
+      <c r="R25" s="16"/>
     </row>
-    <row r="26" spans="1:16" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17"/>
       <c r="B26" s="16"/>
       <c r="C26" s="17"/>
@@ -2612,8 +2725,10 @@
       <c r="N26" s="16"/>
       <c r="O26" s="16"/>
       <c r="P26" s="16"/>
+      <c r="Q26" s="16"/>
+      <c r="R26" s="16"/>
     </row>
-    <row r="27" spans="1:16" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="17"/>
       <c r="B27" s="16"/>
       <c r="C27" s="17"/>
@@ -2630,20 +2745,24 @@
       <c r="N27" s="16"/>
       <c r="O27" s="16"/>
       <c r="P27" s="16"/>
+      <c r="Q27" s="16"/>
+      <c r="R27" s="16"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B28" s="17"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B29" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
     <mergeCell ref="L7:L21"/>
-    <mergeCell ref="P7:P21"/>
+    <mergeCell ref="R7:R21"/>
     <mergeCell ref="C7:C21"/>
     <mergeCell ref="E7:E21"/>
     <mergeCell ref="J7:J21"/>
+    <mergeCell ref="M7:M21"/>
+    <mergeCell ref="Q7:Q21"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
måske ASG kan printes nu..
</commit_message>
<xml_diff>
--- a/Modeller/Agile-Stage-Gate v0.1.xlsx
+++ b/Modeller/Agile-Stage-Gate v0.1.xlsx
@@ -706,8 +706,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1490664" y="2152649"/>
-          <a:ext cx="2111510" cy="1509714"/>
+          <a:off x="1498601" y="2168524"/>
+          <a:ext cx="2095635" cy="1501776"/>
           <a:chOff x="1504951" y="2152649"/>
           <a:chExt cx="2111510" cy="1504951"/>
         </a:xfrm>
@@ -860,8 +860,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5148263" y="2152649"/>
-          <a:ext cx="2114550" cy="1509714"/>
+          <a:off x="5124450" y="2168524"/>
+          <a:ext cx="2098675" cy="1501776"/>
           <a:chOff x="1504951" y="2152649"/>
           <a:chExt cx="2111510" cy="1504951"/>
         </a:xfrm>
@@ -1020,8 +1020,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="11796714" y="2152649"/>
-          <a:ext cx="2111510" cy="1509714"/>
+          <a:off x="11725276" y="2168524"/>
+          <a:ext cx="2079760" cy="1501776"/>
           <a:chOff x="1504951" y="2152649"/>
           <a:chExt cx="2111510" cy="1504951"/>
         </a:xfrm>
@@ -1174,8 +1174,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="17740314" y="2152649"/>
-          <a:ext cx="2111510" cy="1509714"/>
+          <a:off x="17605376" y="2168524"/>
+          <a:ext cx="2095635" cy="1501776"/>
           <a:chOff x="1504951" y="2152649"/>
           <a:chExt cx="2111510" cy="1504951"/>
         </a:xfrm>
@@ -1552,8 +1552,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="25655571" y="2162177"/>
-          <a:ext cx="2111510" cy="1509714"/>
+          <a:off x="25457133" y="2178052"/>
+          <a:ext cx="2095635" cy="1501776"/>
           <a:chOff x="1504951" y="2152649"/>
           <a:chExt cx="2111510" cy="1504951"/>
         </a:xfrm>
@@ -2021,8 +2021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="40" zoomScaleNormal="40" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="40" zoomScalePageLayoutView="50" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2766,7 +2766,10 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="27" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="19" max="1048575" man="1"/>
+  </colBreaks>
   <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Nyt optage frekvenssignal VI
</commit_message>
<xml_diff>
--- a/Modeller/Agile-Stage-Gate v0.1.xlsx
+++ b/Modeller/Agile-Stage-Gate v0.1.xlsx
@@ -706,8 +706,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1498601" y="2168524"/>
-          <a:ext cx="2095635" cy="1501776"/>
+          <a:off x="1490664" y="2152649"/>
+          <a:ext cx="2111510" cy="1509714"/>
           <a:chOff x="1504951" y="2152649"/>
           <a:chExt cx="2111510" cy="1504951"/>
         </a:xfrm>
@@ -860,8 +860,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5124450" y="2168524"/>
-          <a:ext cx="2098675" cy="1501776"/>
+          <a:off x="5148263" y="2152649"/>
+          <a:ext cx="2114550" cy="1509714"/>
           <a:chOff x="1504951" y="2152649"/>
           <a:chExt cx="2111510" cy="1504951"/>
         </a:xfrm>
@@ -1020,8 +1020,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="11725276" y="2168524"/>
-          <a:ext cx="2079760" cy="1501776"/>
+          <a:off x="11796714" y="2152649"/>
+          <a:ext cx="2111510" cy="1509714"/>
           <a:chOff x="1504951" y="2152649"/>
           <a:chExt cx="2111510" cy="1504951"/>
         </a:xfrm>
@@ -1174,8 +1174,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="17605376" y="2168524"/>
-          <a:ext cx="2095635" cy="1501776"/>
+          <a:off x="17740314" y="2152649"/>
+          <a:ext cx="2111510" cy="1509714"/>
           <a:chOff x="1504951" y="2152649"/>
           <a:chExt cx="2111510" cy="1504951"/>
         </a:xfrm>
@@ -1552,8 +1552,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="25457133" y="2178052"/>
-          <a:ext cx="2095635" cy="1501776"/>
+          <a:off x="25655571" y="2162177"/>
+          <a:ext cx="2111510" cy="1509714"/>
           <a:chOff x="1504951" y="2152649"/>
           <a:chExt cx="2111510" cy="1504951"/>
         </a:xfrm>
@@ -2021,8 +2021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V29"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="40" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" zoomScalePageLayoutView="50" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Accepttest tilføjet til tidsplanen
</commit_message>
<xml_diff>
--- a/Modeller/Agile-Stage-Gate v0.1.xlsx
+++ b/Modeller/Agile-Stage-Gate v0.1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="73">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -627,12 +627,6 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="45" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="45"/>
     </xf>
@@ -641,17 +635,23 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="135"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2021,8 +2021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="40" zoomScaleNormal="40" zoomScalePageLayoutView="50" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2131,13 +2131,13 @@
         <v>0</v>
       </c>
       <c r="M5" s="5"/>
-      <c r="N5" s="45" t="s">
+      <c r="N5" s="43" t="s">
         <v>0</v>
       </c>
       <c r="O5" s="7"/>
       <c r="P5" s="7"/>
       <c r="Q5" s="12"/>
-      <c r="R5" s="44" t="s">
+      <c r="R5" s="42" t="s">
         <v>0</v>
       </c>
       <c r="S5" s="24" t="s">
@@ -2184,7 +2184,7 @@
       <c r="L6" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="M6" s="43"/>
+      <c r="M6" s="41"/>
       <c r="N6" s="33" t="s">
         <v>53</v>
       </c>
@@ -2194,7 +2194,7 @@
       <c r="P6" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="Q6" s="43"/>
+      <c r="Q6" s="41"/>
       <c r="R6" s="10" t="s">
         <v>43</v>
       </c>
@@ -2208,13 +2208,13 @@
       <c r="B7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="48" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="42" t="s">
+      <c r="E7" s="48" t="s">
         <v>41</v>
       </c>
       <c r="F7" s="25" t="s">
@@ -2229,16 +2229,16 @@
       <c r="I7" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="J7" s="41" t="s">
+      <c r="J7" s="47" t="s">
         <v>41</v>
       </c>
       <c r="K7" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="L7" s="41" t="s">
+      <c r="L7" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="M7" s="46" t="s">
+      <c r="M7" s="50" t="s">
         <v>71</v>
       </c>
       <c r="N7" s="35" t="s">
@@ -2250,10 +2250,10 @@
       <c r="P7" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="Q7" s="46" t="s">
+      <c r="Q7" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="R7" s="47" t="s">
+      <c r="R7" s="49" t="s">
         <v>44</v>
       </c>
       <c r="S7" s="38"/>
@@ -2263,11 +2263,11 @@
       <c r="B8" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="42"/>
+      <c r="C8" s="48"/>
       <c r="D8" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="42"/>
+      <c r="E8" s="48"/>
       <c r="F8" s="25" t="s">
         <v>30</v>
       </c>
@@ -2280,12 +2280,12 @@
       <c r="I8" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="42"/>
+      <c r="J8" s="48"/>
       <c r="K8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="L8" s="42"/>
-      <c r="M8" s="46"/>
+      <c r="L8" s="48"/>
+      <c r="M8" s="50"/>
       <c r="N8" s="35" t="s">
         <v>55</v>
       </c>
@@ -2295,19 +2295,19 @@
       <c r="P8" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="Q8" s="46"/>
-      <c r="R8" s="47"/>
+      <c r="Q8" s="50"/>
+      <c r="R8" s="49"/>
     </row>
     <row r="9" spans="1:22" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="42"/>
+      <c r="C9" s="48"/>
       <c r="D9" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="42"/>
+      <c r="E9" s="48"/>
       <c r="F9" s="25" t="s">
         <v>37</v>
       </c>
@@ -2316,12 +2316,12 @@
       </c>
       <c r="H9" s="25"/>
       <c r="I9" s="4"/>
-      <c r="J9" s="42"/>
+      <c r="J9" s="48"/>
       <c r="K9" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="L9" s="42"/>
-      <c r="M9" s="46"/>
+      <c r="L9" s="48"/>
+      <c r="M9" s="50"/>
       <c r="N9" s="35" t="s">
         <v>56</v>
       </c>
@@ -2331,31 +2331,31 @@
       <c r="P9" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="Q9" s="46"/>
-      <c r="R9" s="47"/>
+      <c r="Q9" s="50"/>
+      <c r="R9" s="49"/>
     </row>
     <row r="10" spans="1:22" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="42"/>
+      <c r="C10" s="48"/>
       <c r="D10" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="42"/>
+      <c r="E10" s="48"/>
       <c r="F10" s="25" t="s">
         <v>49</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
-      <c r="J10" s="42"/>
+      <c r="J10" s="48"/>
       <c r="K10" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="L10" s="42"/>
-      <c r="M10" s="46"/>
+      <c r="L10" s="48"/>
+      <c r="M10" s="50"/>
       <c r="N10" s="35" t="s">
         <v>57</v>
       </c>
@@ -2365,29 +2365,29 @@
       <c r="P10" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="Q10" s="46"/>
-      <c r="R10" s="47"/>
+      <c r="Q10" s="50"/>
+      <c r="R10" s="49"/>
     </row>
     <row r="11" spans="1:22" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="42"/>
+      <c r="C11" s="48"/>
       <c r="D11" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="42"/>
+      <c r="E11" s="48"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
-      <c r="J11" s="42"/>
+      <c r="J11" s="48"/>
       <c r="K11" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="L11" s="42"/>
-      <c r="M11" s="46"/>
+      <c r="L11" s="48"/>
+      <c r="M11" s="50"/>
       <c r="N11" s="35" t="s">
         <v>58</v>
       </c>
@@ -2397,27 +2397,27 @@
       <c r="P11" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="Q11" s="46"/>
-      <c r="R11" s="47"/>
+      <c r="Q11" s="50"/>
+      <c r="R11" s="49"/>
     </row>
     <row r="12" spans="1:22" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="42"/>
+      <c r="C12" s="48"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="42"/>
+      <c r="E12" s="48"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
-      <c r="J12" s="42"/>
+      <c r="J12" s="48"/>
       <c r="K12" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="L12" s="42"/>
-      <c r="M12" s="46"/>
+      <c r="L12" s="48"/>
+      <c r="M12" s="50"/>
       <c r="N12" s="35" t="s">
         <v>59</v>
       </c>
@@ -2427,226 +2427,228 @@
       <c r="P12" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="Q12" s="46"/>
-      <c r="R12" s="47"/>
+      <c r="Q12" s="50"/>
+      <c r="R12" s="49"/>
     </row>
     <row r="13" spans="1:22" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="42"/>
+      <c r="C13" s="48"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="42"/>
+      <c r="E13" s="48"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
-      <c r="J13" s="42"/>
+      <c r="J13" s="48"/>
       <c r="K13" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="L13" s="42"/>
-      <c r="M13" s="46"/>
+      <c r="L13" s="48"/>
+      <c r="M13" s="50"/>
       <c r="N13" s="35" t="s">
         <v>60</v>
       </c>
       <c r="O13" s="35"/>
       <c r="P13" s="35"/>
-      <c r="Q13" s="46"/>
-      <c r="R13" s="47"/>
+      <c r="Q13" s="50"/>
+      <c r="R13" s="49"/>
     </row>
     <row r="14" spans="1:22" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="42"/>
+      <c r="C14" s="48"/>
       <c r="D14" s="4"/>
-      <c r="E14" s="42"/>
+      <c r="E14" s="48"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
-      <c r="J14" s="42"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="42"/>
-      <c r="M14" s="46"/>
+      <c r="J14" s="48"/>
+      <c r="K14" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="L14" s="48"/>
+      <c r="M14" s="50"/>
       <c r="N14" s="35" t="s">
         <v>61</v>
       </c>
       <c r="O14" s="4"/>
       <c r="P14" s="35"/>
-      <c r="Q14" s="46"/>
-      <c r="R14" s="47"/>
+      <c r="Q14" s="50"/>
+      <c r="R14" s="49"/>
     </row>
     <row r="15" spans="1:22" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="42"/>
+      <c r="C15" s="48"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="42"/>
+      <c r="E15" s="48"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
-      <c r="J15" s="42"/>
+      <c r="J15" s="48"/>
       <c r="K15" s="4"/>
-      <c r="L15" s="42"/>
-      <c r="M15" s="46"/>
+      <c r="L15" s="48"/>
+      <c r="M15" s="50"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
       <c r="P15" s="35"/>
-      <c r="Q15" s="46"/>
-      <c r="R15" s="47"/>
+      <c r="Q15" s="50"/>
+      <c r="R15" s="49"/>
     </row>
     <row r="16" spans="1:22" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="42"/>
+      <c r="C16" s="48"/>
       <c r="D16" s="4"/>
-      <c r="E16" s="42"/>
+      <c r="E16" s="48"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
-      <c r="J16" s="42"/>
+      <c r="J16" s="48"/>
       <c r="K16" s="4"/>
-      <c r="L16" s="42"/>
-      <c r="M16" s="46"/>
+      <c r="L16" s="48"/>
+      <c r="M16" s="50"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
       <c r="P16" s="35"/>
-      <c r="Q16" s="46"/>
-      <c r="R16" s="47"/>
+      <c r="Q16" s="50"/>
+      <c r="R16" s="49"/>
     </row>
     <row r="17" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="42"/>
+      <c r="C17" s="48"/>
       <c r="D17" s="4"/>
-      <c r="E17" s="42"/>
+      <c r="E17" s="48"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
-      <c r="J17" s="42"/>
+      <c r="J17" s="48"/>
       <c r="K17" s="4"/>
-      <c r="L17" s="42"/>
-      <c r="M17" s="46"/>
+      <c r="L17" s="48"/>
+      <c r="M17" s="50"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
-      <c r="Q17" s="46"/>
-      <c r="R17" s="47"/>
+      <c r="Q17" s="50"/>
+      <c r="R17" s="49"/>
     </row>
     <row r="18" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="42"/>
+      <c r="C18" s="48"/>
       <c r="D18" s="4"/>
-      <c r="E18" s="42"/>
+      <c r="E18" s="48"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
-      <c r="J18" s="42"/>
+      <c r="J18" s="48"/>
       <c r="K18" s="4"/>
-      <c r="L18" s="42"/>
-      <c r="M18" s="46"/>
+      <c r="L18" s="48"/>
+      <c r="M18" s="50"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
-      <c r="Q18" s="46"/>
-      <c r="R18" s="47"/>
+      <c r="Q18" s="50"/>
+      <c r="R18" s="49"/>
     </row>
     <row r="19" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="4"/>
-      <c r="C19" s="42"/>
+      <c r="C19" s="48"/>
       <c r="D19" s="4"/>
-      <c r="E19" s="42"/>
+      <c r="E19" s="48"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
-      <c r="J19" s="42"/>
+      <c r="J19" s="48"/>
       <c r="K19" s="4"/>
-      <c r="L19" s="42"/>
-      <c r="M19" s="46"/>
+      <c r="L19" s="48"/>
+      <c r="M19" s="50"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
-      <c r="Q19" s="46"/>
-      <c r="R19" s="47"/>
+      <c r="Q19" s="50"/>
+      <c r="R19" s="49"/>
     </row>
     <row r="20" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="4"/>
-      <c r="C20" s="42"/>
+      <c r="C20" s="48"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="42"/>
+      <c r="E20" s="48"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
-      <c r="J20" s="42"/>
+      <c r="J20" s="48"/>
       <c r="K20" s="4"/>
-      <c r="L20" s="42"/>
-      <c r="M20" s="46"/>
+      <c r="L20" s="48"/>
+      <c r="M20" s="50"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
-      <c r="Q20" s="46"/>
-      <c r="R20" s="47"/>
+      <c r="Q20" s="50"/>
+      <c r="R20" s="49"/>
     </row>
     <row r="21" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
-      <c r="B21" s="48"/>
-      <c r="C21" s="42"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="48"/>
-      <c r="I21" s="48"/>
-      <c r="J21" s="42"/>
-      <c r="K21" s="48"/>
-      <c r="L21" s="42"/>
-      <c r="M21" s="46"/>
-      <c r="N21" s="48"/>
-      <c r="O21" s="48"/>
-      <c r="P21" s="48"/>
-      <c r="Q21" s="46"/>
-      <c r="R21" s="47"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="44"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="44"/>
+      <c r="J21" s="48"/>
+      <c r="K21" s="44"/>
+      <c r="L21" s="48"/>
+      <c r="M21" s="50"/>
+      <c r="N21" s="44"/>
+      <c r="O21" s="44"/>
+      <c r="P21" s="44"/>
+      <c r="Q21" s="50"/>
+      <c r="R21" s="49"/>
     </row>
     <row r="22" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="49"/>
-      <c r="B22" s="49"/>
-      <c r="C22" s="50"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="49"/>
-      <c r="F22" s="49"/>
-      <c r="G22" s="49"/>
-      <c r="H22" s="49"/>
-      <c r="I22" s="49"/>
-      <c r="J22" s="49"/>
-      <c r="K22" s="49"/>
-      <c r="L22" s="49"/>
-      <c r="M22" s="49"/>
-      <c r="N22" s="49"/>
-      <c r="O22" s="49"/>
-      <c r="P22" s="49"/>
-      <c r="Q22" s="49"/>
-      <c r="R22" s="49"/>
+      <c r="A22" s="45"/>
+      <c r="B22" s="45"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="45"/>
+      <c r="I22" s="45"/>
+      <c r="J22" s="45"/>
+      <c r="K22" s="45"/>
+      <c r="L22" s="45"/>
+      <c r="M22" s="45"/>
+      <c r="N22" s="45"/>
+      <c r="O22" s="45"/>
+      <c r="P22" s="45"/>
+      <c r="Q22" s="45"/>
+      <c r="R22" s="45"/>
     </row>
     <row r="23" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17"/>

</xml_diff>

<commit_message>
Stage Gate + Agil Stage Gate er fikset og indkluderet i Projektrapporten
</commit_message>
<xml_diff>
--- a/Modeller/Agile-Stage-Gate v0.1.xlsx
+++ b/Modeller/Agile-Stage-Gate v0.1.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jannie\Documents\GitHub\BachelorprojektBravo\Modeller\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="15525" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15280" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Agil Stage-Gate" sheetId="1" r:id="rId1"/>
+    <sheet name="Konceptudvikling tjekliste" sheetId="2" r:id="rId2"/>
+    <sheet name="High-level produkts. tjekliste " sheetId="3" r:id="rId3"/>
+    <sheet name="Udviklingsfase tjekliste   " sheetId="4" r:id="rId4"/>
+    <sheet name="Implementering tjekliste" sheetId="5" r:id="rId5"/>
+    <sheet name="Projektrapport tjekliste" sheetId="6" r:id="rId6"/>
+    <sheet name="Dokumentationsrapport tjekliste" sheetId="7" r:id="rId7"/>
+    <sheet name="Procesrapport tjekliste" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="88">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -80,9 +82,6 @@
     <t>Planlægning af litteratursøgning</t>
   </si>
   <si>
-    <t>High-level produktspecifikation</t>
-  </si>
-  <si>
     <t>Litteratursøgning</t>
   </si>
   <si>
@@ -243,13 +242,61 @@
   </si>
   <si>
     <t>Review 12.12.2016</t>
+  </si>
+  <si>
+    <t>Konceptudvikling tjekliste</t>
+  </si>
+  <si>
+    <t>High-level produktspecifikation tjekliste</t>
+  </si>
+  <si>
+    <t>Udviklingsfase tjekliste</t>
+  </si>
+  <si>
+    <t>Implementering tjekliste</t>
+  </si>
+  <si>
+    <t>Projektrapport    tjekliste</t>
+  </si>
+  <si>
+    <t>Dokumentations-             rapport tjekliste</t>
+  </si>
+  <si>
+    <t>Procesrapport        tjekliste</t>
+  </si>
+  <si>
+    <t>High-level produkt-       specifikation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                   Signatures</t>
+  </si>
+  <si>
+    <t>Gates</t>
+  </si>
+  <si>
+    <t>Stages</t>
+  </si>
+  <si>
+    <t>Reviews</t>
+  </si>
+  <si>
+    <t>Approved</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> w/Conditions</t>
+  </si>
+  <si>
+    <t>Rejected</t>
+  </si>
+  <si>
+    <t>Not Applicable</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -313,8 +360,48 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -339,8 +426,50 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5B9BD5"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF595959"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCF305"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDD0806"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -482,14 +611,14 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -497,35 +626,112 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="135"/>
@@ -596,9 +802,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="45" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -636,11 +839,28 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="135"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -653,12 +873,73 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection hidden="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
-    <cellStyle name="Besøgt link" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
+  <cellStyles count="17">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -706,8 +987,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1490664" y="2152649"/>
-          <a:ext cx="2111510" cy="1509714"/>
+          <a:off x="1511301" y="2178049"/>
+          <a:ext cx="2105160" cy="1524001"/>
           <a:chOff x="1504951" y="2152649"/>
           <a:chExt cx="2111510" cy="1504951"/>
         </a:xfrm>
@@ -860,8 +1141,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5148263" y="2152649"/>
-          <a:ext cx="2114550" cy="1509714"/>
+          <a:off x="5156200" y="2178049"/>
+          <a:ext cx="2108200" cy="1524001"/>
           <a:chOff x="1504951" y="2152649"/>
           <a:chExt cx="2111510" cy="1504951"/>
         </a:xfrm>
@@ -1020,8 +1301,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="11796714" y="2152649"/>
-          <a:ext cx="2111510" cy="1509714"/>
+          <a:off x="11785601" y="2178049"/>
+          <a:ext cx="2098810" cy="1524001"/>
           <a:chOff x="1504951" y="2152649"/>
           <a:chExt cx="2111510" cy="1504951"/>
         </a:xfrm>
@@ -1174,8 +1455,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="17740314" y="2152649"/>
-          <a:ext cx="2111510" cy="1509714"/>
+          <a:off x="17703801" y="2178049"/>
+          <a:ext cx="2105160" cy="1524001"/>
           <a:chOff x="1504951" y="2152649"/>
           <a:chExt cx="2111510" cy="1504951"/>
         </a:xfrm>
@@ -1552,8 +1833,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="25655571" y="2162177"/>
-          <a:ext cx="2111510" cy="1509714"/>
+          <a:off x="25593658" y="2187577"/>
+          <a:ext cx="2105160" cy="1524001"/>
           <a:chOff x="1504951" y="2152649"/>
           <a:chExt cx="2111510" cy="1504951"/>
         </a:xfrm>
@@ -2021,22 +2302,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="40" zoomScaleNormal="40" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="F7" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="50" workbookViewId="0">
+      <selection activeCell="T17" sqref="T17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.125" customWidth="1"/>
-    <col min="2" max="12" width="23.625" customWidth="1"/>
-    <col min="13" max="13" width="23.625" style="17" customWidth="1"/>
-    <col min="14" max="16" width="23.625" customWidth="1"/>
-    <col min="17" max="17" width="23.625" style="17" customWidth="1"/>
-    <col min="18" max="20" width="23.625" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" customWidth="1"/>
+    <col min="2" max="12" width="23.6640625" customWidth="1"/>
+    <col min="13" max="13" width="23.6640625" style="17" customWidth="1"/>
+    <col min="14" max="16" width="23.6640625" customWidth="1"/>
+    <col min="17" max="17" width="23.6640625" style="17" customWidth="1"/>
+    <col min="18" max="20" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="48.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:22" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="49" customHeight="1"/>
+    <row r="2" spans="1:22" ht="102" customHeight="1">
       <c r="A2" s="19"/>
       <c r="B2" s="20" t="s">
         <v>4</v>
@@ -2059,7 +2340,7 @@
       <c r="R2" s="21"/>
       <c r="S2" s="22"/>
     </row>
-    <row r="3" spans="1:22" ht="68.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" ht="68" customHeight="1">
       <c r="A3" s="17"/>
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
@@ -2078,7 +2359,7 @@
       <c r="R3" s="17"/>
       <c r="S3" s="17"/>
     </row>
-    <row r="4" spans="1:22" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" ht="69" customHeight="1">
       <c r="A4" s="16"/>
       <c r="B4" s="17"/>
       <c r="C4" s="17"/>
@@ -2097,7 +2378,7 @@
       <c r="R4" s="17"/>
       <c r="S4" s="17"/>
     </row>
-    <row r="5" spans="1:22" ht="113.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" ht="113" customHeight="1">
       <c r="A5" s="23"/>
       <c r="B5" s="24"/>
       <c r="C5" s="12" t="s">
@@ -2131,13 +2412,13 @@
         <v>0</v>
       </c>
       <c r="M5" s="5"/>
-      <c r="N5" s="43" t="s">
+      <c r="N5" s="42" t="s">
         <v>0</v>
       </c>
       <c r="O5" s="7"/>
       <c r="P5" s="7"/>
       <c r="Q5" s="12"/>
-      <c r="R5" s="42" t="s">
+      <c r="R5" s="41" t="s">
         <v>0</v>
       </c>
       <c r="S5" s="24" t="s">
@@ -2149,7 +2430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="141.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" ht="142" customHeight="1">
       <c r="A6" s="8"/>
       <c r="B6" s="29" t="s">
         <v>1</v>
@@ -2157,8 +2438,8 @@
       <c r="C6" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="30" t="s">
-        <v>18</v>
+      <c r="D6" s="50" t="s">
+        <v>79</v>
       </c>
       <c r="E6" s="27" t="s">
         <v>14</v>
@@ -2175,482 +2456,524 @@
       <c r="I6" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="32" t="s">
-        <v>42</v>
+      <c r="J6" s="31" t="s">
+        <v>41</v>
       </c>
       <c r="K6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L6" s="39" t="s">
-        <v>70</v>
-      </c>
-      <c r="M6" s="41"/>
-      <c r="N6" s="33" t="s">
+      <c r="L6" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="M6" s="40"/>
+      <c r="N6" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="O6" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="P6" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="O6" s="40" t="s">
-        <v>69</v>
-      </c>
-      <c r="P6" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q6" s="41"/>
+      <c r="Q6" s="40"/>
       <c r="R6" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="S6" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="S6" s="36" t="s">
         <v>0</v>
       </c>
       <c r="T6" s="3"/>
     </row>
-    <row r="7" spans="1:22" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" ht="57" customHeight="1">
       <c r="A7" s="8"/>
       <c r="B7" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="48" t="s">
-        <v>26</v>
+        <v>20</v>
+      </c>
+      <c r="C7" s="52" t="s">
+        <v>25</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="48" t="s">
-        <v>41</v>
+        <v>18</v>
+      </c>
+      <c r="E7" s="52" t="s">
+        <v>40</v>
       </c>
       <c r="F7" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="25" t="s">
-        <v>32</v>
-      </c>
       <c r="H7" s="25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I7" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="J7" s="47" t="s">
-        <v>41</v>
+        <v>37</v>
+      </c>
+      <c r="J7" s="51" t="s">
+        <v>40</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="L7" s="47" t="s">
-        <v>68</v>
-      </c>
-      <c r="M7" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="L7" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="M7" s="54" t="s">
+        <v>70</v>
+      </c>
+      <c r="N7" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="O7" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="P7" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q7" s="54" t="s">
         <v>71</v>
       </c>
-      <c r="N7" s="35" t="s">
-        <v>52</v>
-      </c>
-      <c r="O7" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="P7" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q7" s="50" t="s">
-        <v>72</v>
-      </c>
-      <c r="R7" s="49" t="s">
-        <v>44</v>
-      </c>
-      <c r="S7" s="38"/>
+      <c r="R7" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="S7" s="37"/>
     </row>
-    <row r="8" spans="1:22" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" ht="57" customHeight="1">
       <c r="A8" s="8"/>
       <c r="B8" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="48"/>
+        <v>19</v>
+      </c>
+      <c r="C8" s="52"/>
       <c r="D8" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="48"/>
+      <c r="E8" s="52"/>
       <c r="F8" s="25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G8" s="25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H8" s="25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I8" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="J8" s="48"/>
+        <v>38</v>
+      </c>
+      <c r="J8" s="52"/>
       <c r="K8" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="L8" s="48"/>
-      <c r="M8" s="50"/>
-      <c r="N8" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="O8" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="L8" s="52"/>
+      <c r="M8" s="54"/>
+      <c r="N8" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="O8" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="P8" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="P8" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q8" s="50"/>
-      <c r="R8" s="49"/>
+      <c r="Q8" s="54"/>
+      <c r="R8" s="53"/>
     </row>
-    <row r="9" spans="1:22" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" ht="57" customHeight="1">
       <c r="A9" s="8"/>
       <c r="B9" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="48"/>
+        <v>23</v>
+      </c>
+      <c r="C9" s="52"/>
       <c r="D9" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="48"/>
+      <c r="E9" s="52"/>
       <c r="F9" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G9" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H9" s="25"/>
       <c r="I9" s="4"/>
-      <c r="J9" s="48"/>
+      <c r="J9" s="52"/>
       <c r="K9" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="L9" s="48"/>
-      <c r="M9" s="50"/>
-      <c r="N9" s="35" t="s">
-        <v>56</v>
-      </c>
-      <c r="O9" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="L9" s="52"/>
+      <c r="M9" s="54"/>
+      <c r="N9" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="O9" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="P9" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q9" s="50"/>
-      <c r="R9" s="49"/>
+      <c r="P9" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q9" s="54"/>
+      <c r="R9" s="53"/>
     </row>
-    <row r="10" spans="1:22" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" ht="57" customHeight="1">
       <c r="A10" s="8"/>
       <c r="B10" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="48"/>
+        <v>27</v>
+      </c>
+      <c r="C10" s="52"/>
       <c r="D10" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="48"/>
+        <v>26</v>
+      </c>
+      <c r="E10" s="52"/>
       <c r="F10" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
-      <c r="J10" s="48"/>
+      <c r="J10" s="52"/>
       <c r="K10" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="L10" s="48"/>
-      <c r="M10" s="50"/>
-      <c r="N10" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="O10" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="L10" s="52"/>
+      <c r="M10" s="54"/>
+      <c r="N10" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="O10" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="P10" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q10" s="50"/>
-      <c r="R10" s="49"/>
+      <c r="P10" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q10" s="54"/>
+      <c r="R10" s="53"/>
     </row>
-    <row r="11" spans="1:22" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" ht="57" customHeight="1" thickBot="1">
       <c r="A11" s="8"/>
       <c r="B11" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="48"/>
+        <v>28</v>
+      </c>
+      <c r="C11" s="52"/>
       <c r="D11" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="48"/>
+      <c r="E11" s="52"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
-      <c r="J11" s="48"/>
+      <c r="J11" s="52"/>
       <c r="K11" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="L11" s="48"/>
-      <c r="M11" s="50"/>
-      <c r="N11" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="O11" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="L11" s="52"/>
+      <c r="M11" s="54"/>
+      <c r="N11" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="O11" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="P11" s="35" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q11" s="50"/>
-      <c r="R11" s="49"/>
+      <c r="P11" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q11" s="54"/>
+      <c r="R11" s="53"/>
+      <c r="T11" s="58" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="12" spans="1:22" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" ht="57" customHeight="1">
       <c r="A12" s="8"/>
       <c r="B12" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="48"/>
+        <v>21</v>
+      </c>
+      <c r="C12" s="52"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="48"/>
+      <c r="E12" s="52"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
-      <c r="J12" s="48"/>
+      <c r="J12" s="52"/>
       <c r="K12" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="L12" s="48"/>
-      <c r="M12" s="50"/>
-      <c r="N12" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="O12" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="P12" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q12" s="50"/>
-      <c r="R12" s="49"/>
+        <v>49</v>
+      </c>
+      <c r="L12" s="52"/>
+      <c r="M12" s="54"/>
+      <c r="N12" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="O12" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="P12" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q12" s="54"/>
+      <c r="R12" s="53"/>
+      <c r="T12" s="59" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="13" spans="1:22" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" ht="57" customHeight="1">
       <c r="A13" s="8"/>
       <c r="B13" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="48"/>
+      <c r="C13" s="52"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="48"/>
+      <c r="E13" s="52"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
-      <c r="J13" s="48"/>
+      <c r="J13" s="52"/>
       <c r="K13" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="L13" s="48"/>
-      <c r="M13" s="50"/>
-      <c r="N13" s="35" t="s">
-        <v>60</v>
-      </c>
-      <c r="O13" s="35"/>
-      <c r="P13" s="35"/>
-      <c r="Q13" s="50"/>
-      <c r="R13" s="49"/>
+        <v>50</v>
+      </c>
+      <c r="L13" s="52"/>
+      <c r="M13" s="54"/>
+      <c r="N13" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="O13" s="34"/>
+      <c r="P13" s="34"/>
+      <c r="Q13" s="54"/>
+      <c r="R13" s="53"/>
+      <c r="T13" s="60" t="s">
+        <v>82</v>
+      </c>
     </row>
-    <row r="14" spans="1:22" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" ht="57" customHeight="1">
       <c r="A14" s="8"/>
       <c r="B14" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="48"/>
+        <v>22</v>
+      </c>
+      <c r="C14" s="52"/>
       <c r="D14" s="4"/>
-      <c r="E14" s="48"/>
+      <c r="E14" s="52"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
-      <c r="J14" s="48"/>
+      <c r="J14" s="52"/>
       <c r="K14" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="L14" s="48"/>
-      <c r="M14" s="50"/>
-      <c r="N14" s="35" t="s">
-        <v>61</v>
+      <c r="L14" s="52"/>
+      <c r="M14" s="54"/>
+      <c r="N14" s="34" t="s">
+        <v>60</v>
       </c>
       <c r="O14" s="4"/>
-      <c r="P14" s="35"/>
-      <c r="Q14" s="50"/>
-      <c r="R14" s="49"/>
+      <c r="P14" s="34"/>
+      <c r="Q14" s="54"/>
+      <c r="R14" s="53"/>
+      <c r="T14" s="61" t="s">
+        <v>83</v>
+      </c>
     </row>
-    <row r="15" spans="1:22" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" ht="57" customHeight="1">
       <c r="A15" s="8"/>
-      <c r="B15" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="48"/>
+      <c r="B15" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="52"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="48"/>
+      <c r="E15" s="52"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
-      <c r="J15" s="48"/>
+      <c r="J15" s="52"/>
       <c r="K15" s="4"/>
-      <c r="L15" s="48"/>
-      <c r="M15" s="50"/>
+      <c r="L15" s="52"/>
+      <c r="M15" s="54"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
-      <c r="P15" s="35"/>
-      <c r="Q15" s="50"/>
-      <c r="R15" s="49"/>
+      <c r="P15" s="34"/>
+      <c r="Q15" s="54"/>
+      <c r="R15" s="53"/>
+      <c r="T15" s="62" t="s">
+        <v>84</v>
+      </c>
     </row>
-    <row r="16" spans="1:22" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" ht="57" customHeight="1">
       <c r="A16" s="8"/>
       <c r="B16" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="48"/>
+      <c r="C16" s="52"/>
       <c r="D16" s="4"/>
-      <c r="E16" s="48"/>
+      <c r="E16" s="52"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
-      <c r="J16" s="48"/>
+      <c r="J16" s="52"/>
       <c r="K16" s="4"/>
-      <c r="L16" s="48"/>
-      <c r="M16" s="50"/>
+      <c r="L16" s="52"/>
+      <c r="M16" s="54"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
-      <c r="P16" s="35"/>
-      <c r="Q16" s="50"/>
-      <c r="R16" s="49"/>
+      <c r="P16" s="34"/>
+      <c r="Q16" s="54"/>
+      <c r="R16" s="53"/>
+      <c r="T16" s="63" t="s">
+        <v>84</v>
+      </c>
     </row>
-    <row r="17" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" ht="57" customHeight="1">
       <c r="A17" s="8"/>
       <c r="B17" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="48"/>
+      <c r="C17" s="52"/>
       <c r="D17" s="4"/>
-      <c r="E17" s="48"/>
+      <c r="E17" s="52"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
-      <c r="J17" s="48"/>
+      <c r="J17" s="52"/>
       <c r="K17" s="4"/>
-      <c r="L17" s="48"/>
-      <c r="M17" s="50"/>
+      <c r="L17" s="52"/>
+      <c r="M17" s="54"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
-      <c r="Q17" s="50"/>
-      <c r="R17" s="49"/>
+      <c r="Q17" s="54"/>
+      <c r="R17" s="53"/>
+      <c r="T17" s="64" t="s">
+        <v>85</v>
+      </c>
     </row>
-    <row r="18" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" ht="57" customHeight="1">
       <c r="A18" s="8"/>
       <c r="B18" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="48"/>
+      <c r="C18" s="52"/>
       <c r="D18" s="4"/>
-      <c r="E18" s="48"/>
+      <c r="E18" s="52"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
-      <c r="J18" s="48"/>
+      <c r="J18" s="52"/>
       <c r="K18" s="4"/>
-      <c r="L18" s="48"/>
-      <c r="M18" s="50"/>
+      <c r="L18" s="52"/>
+      <c r="M18" s="54"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
-      <c r="Q18" s="50"/>
-      <c r="R18" s="49"/>
+      <c r="Q18" s="54"/>
+      <c r="R18" s="53"/>
+      <c r="T18" s="65" t="s">
+        <v>86</v>
+      </c>
     </row>
-    <row r="19" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" ht="57" customHeight="1" thickBot="1">
       <c r="A19" s="8"/>
       <c r="B19" s="4"/>
-      <c r="C19" s="48"/>
+      <c r="C19" s="52"/>
       <c r="D19" s="4"/>
-      <c r="E19" s="48"/>
+      <c r="E19" s="52"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
-      <c r="J19" s="48"/>
+      <c r="J19" s="52"/>
       <c r="K19" s="4"/>
-      <c r="L19" s="48"/>
-      <c r="M19" s="50"/>
+      <c r="L19" s="52"/>
+      <c r="M19" s="54"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
-      <c r="Q19" s="50"/>
-      <c r="R19" s="49"/>
+      <c r="Q19" s="54"/>
+      <c r="R19" s="53"/>
+      <c r="T19" s="66" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="20" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" ht="57" customHeight="1">
       <c r="A20" s="8"/>
       <c r="B20" s="4"/>
-      <c r="C20" s="48"/>
+      <c r="C20" s="52"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="48"/>
+      <c r="E20" s="52"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
-      <c r="J20" s="48"/>
+      <c r="J20" s="52"/>
       <c r="K20" s="4"/>
-      <c r="L20" s="48"/>
-      <c r="M20" s="50"/>
+      <c r="L20" s="52"/>
+      <c r="M20" s="54"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
-      <c r="Q20" s="50"/>
-      <c r="R20" s="49"/>
+      <c r="Q20" s="54"/>
+      <c r="R20" s="53"/>
+      <c r="T20" s="67"/>
     </row>
-    <row r="21" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" ht="57" customHeight="1">
       <c r="A21" s="8"/>
-      <c r="B21" s="44"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="44"/>
-      <c r="G21" s="44"/>
-      <c r="H21" s="44"/>
-      <c r="I21" s="44"/>
-      <c r="J21" s="48"/>
-      <c r="K21" s="44"/>
-      <c r="L21" s="48"/>
-      <c r="M21" s="50"/>
-      <c r="N21" s="44"/>
-      <c r="O21" s="44"/>
-      <c r="P21" s="44"/>
-      <c r="Q21" s="50"/>
-      <c r="R21" s="49"/>
+      <c r="B21" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="52"/>
+      <c r="D21" s="46" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" s="52"/>
+      <c r="F21" s="55" t="s">
+        <v>74</v>
+      </c>
+      <c r="G21" s="56"/>
+      <c r="H21" s="56"/>
+      <c r="I21" s="57"/>
+      <c r="J21" s="52"/>
+      <c r="K21" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="L21" s="52"/>
+      <c r="M21" s="54"/>
+      <c r="N21" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="O21" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="P21" s="48" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q21" s="54"/>
+      <c r="R21" s="53"/>
     </row>
-    <row r="22" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="45"/>
-      <c r="B22" s="45"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="45"/>
-      <c r="G22" s="45"/>
-      <c r="H22" s="45"/>
-      <c r="I22" s="45"/>
-      <c r="J22" s="45"/>
-      <c r="K22" s="45"/>
-      <c r="L22" s="45"/>
-      <c r="M22" s="45"/>
-      <c r="N22" s="45"/>
-      <c r="O22" s="45"/>
-      <c r="P22" s="45"/>
-      <c r="Q22" s="45"/>
-      <c r="R22" s="45"/>
+    <row r="22" spans="1:20" ht="57" customHeight="1">
+      <c r="A22" s="43"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="43"/>
+      <c r="K22" s="43"/>
+      <c r="L22" s="43"/>
+      <c r="M22" s="43"/>
+      <c r="N22" s="43"/>
+      <c r="O22" s="43"/>
+      <c r="P22" s="43"/>
+      <c r="Q22" s="43"/>
+      <c r="R22" s="43"/>
     </row>
-    <row r="23" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" ht="57" customHeight="1">
       <c r="A23" s="17"/>
       <c r="B23" s="16"/>
       <c r="C23" s="18"/>
@@ -2670,7 +2993,7 @@
       <c r="Q23" s="16"/>
       <c r="R23" s="16"/>
     </row>
-    <row r="24" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" ht="57" customHeight="1">
       <c r="A24" s="17"/>
       <c r="B24" s="16"/>
       <c r="C24" s="18"/>
@@ -2690,7 +3013,7 @@
       <c r="Q24" s="16"/>
       <c r="R24" s="16"/>
     </row>
-    <row r="25" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" ht="57" customHeight="1">
       <c r="A25" s="17"/>
       <c r="B25" s="16"/>
       <c r="C25" s="18"/>
@@ -2710,7 +3033,7 @@
       <c r="Q25" s="16"/>
       <c r="R25" s="16"/>
     </row>
-    <row r="26" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" ht="57" customHeight="1">
       <c r="A26" s="17"/>
       <c r="B26" s="16"/>
       <c r="C26" s="17"/>
@@ -2730,7 +3053,7 @@
       <c r="Q26" s="16"/>
       <c r="R26" s="16"/>
     </row>
-    <row r="27" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" ht="57" customHeight="1">
       <c r="A27" s="17"/>
       <c r="B27" s="16"/>
       <c r="C27" s="17"/>
@@ -2750,14 +3073,14 @@
       <c r="Q27" s="16"/>
       <c r="R27" s="16"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20">
       <c r="B28" s="17"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20">
       <c r="B29" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="L7:L21"/>
     <mergeCell ref="R7:R21"/>
     <mergeCell ref="C7:C21"/>
@@ -2765,14 +3088,158 @@
     <mergeCell ref="J7:J21"/>
     <mergeCell ref="M7:M21"/>
     <mergeCell ref="Q7:Q21"/>
+    <mergeCell ref="F21:I21"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" scale="27" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="27" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="19" max="1048575" man="1"/>
   </colBreaks>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A70"/>
+  <sheetViews>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="70" spans="1:1">
+      <c r="A70" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>